<commit_message>
Change to load Google Spreadsheet.
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="98">
   <si>
     <t>ID</t>
   </si>
@@ -64,12 +64,18 @@
     <t>https://www.cloudskillsboost.google/public_profiles/a98b610a-b81e-44c5-8625-3ff5e0cc3146</t>
   </si>
   <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/ff00dd6d-bcd5-4625-82dc-65bde721e703</t>
+  </si>
+  <si>
     <t>https://www.cloudskillsboost.google/public_profiles/706c9f48-d96c-40e0-bcaa-0df3f60305c9</t>
   </si>
   <si>
     <t>https://www.cloudskillsboost.google/public_profiles/1ab53805-4630-4b28-a63b-bdbb6004e6be</t>
   </si>
   <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/13eafb69-7319-45b7-8b8a-171fcda69bd0</t>
+  </si>
+  <si>
     <t>https://www.cloudskillsboost.google/public_profiles/23724295-6614-4d5d-86a9-00ccd963e47c</t>
   </si>
   <si>
@@ -85,10 +91,13 @@
     <t>https://www.cloudskillsboost.google/public_profiles/e70d73e2-e8ed-4d29-8193-56b4c0a2fc15</t>
   </si>
   <si>
+    <t>https://www.cloudskillsboost.google/public_profiles/da9d823c-b17f-434c-b862-055e7ace088c</t>
+  </si>
+  <si>
     <t>https://www.cloudskillsboost.google/public_profiles/31c67f03-0a43-4194-8c23-3dde40674561</t>
   </si>
   <si>
-    <t>https://www.cloudskillsboost.google/public_profiles/a03a4b08-27bc-49c4-910c-42251eacaae4</t>
+    <t>https://www.cloudskillsboost.google/public_profiles/e23b84f1-dede-4bb6-91bb-eeca0297d4ea</t>
   </si>
   <si>
     <t>https://www.cloudskillsboost.google/public_profiles/3dea8479-29e3-4df7-8e6d-94e57404a27e</t>
@@ -676,7 +685,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -752,19 +761,19 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -778,22 +787,22 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -807,22 +816,22 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -838,52 +847,70 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B9">
-        <v>220019902</v>
+        <v>220018014</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B10">
-        <v>220046953</v>
+        <v>220019902</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B11">
-        <v>220066903</v>
+        <v>220046953</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B12">
-        <v>220068459</v>
+        <v>220055950</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>18</v>
@@ -891,41 +918,35 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B13">
-        <v>220070191</v>
+        <v>220066903</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B14">
-        <v>220072750</v>
+        <v>220068459</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="B15">
-        <v>220073549</v>
+        <v>220070191</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>21</v>
@@ -933,21 +954,30 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B16">
-        <v>220093930</v>
+        <v>220072750</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="E16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B17">
-        <v>220106745</v>
+        <v>220073549</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>23</v>
@@ -955,30 +985,21 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B18">
-        <v>220110802</v>
+        <v>220086336</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19">
-        <v>220126676</v>
+        <v>220093930</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>25</v>
@@ -986,10 +1007,10 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B20">
-        <v>220131060</v>
+        <v>220106745</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>26</v>
@@ -997,21 +1018,30 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B21">
-        <v>220131698</v>
+        <v>220110802</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="E21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B22">
-        <v>220133606</v>
+        <v>220126676</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>28</v>
@@ -1019,10 +1049,10 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>220133692</v>
+        <v>220131060</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>29</v>
@@ -1030,33 +1060,21 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B24">
-        <v>220145273</v>
+        <v>220131698</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D24" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" t="s">
-        <v>46</v>
-      </c>
-      <c r="F24" t="s">
-        <v>46</v>
-      </c>
-      <c r="I24" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B25">
-        <v>220212622</v>
+        <v>220133606</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>31</v>
@@ -1064,115 +1082,130 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B26">
-        <v>220224633</v>
+        <v>220133692</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E26" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B27">
-        <v>220237051</v>
+        <v>220145273</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E27" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F27" t="s">
-        <v>46</v>
-      </c>
-      <c r="G27" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H27" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I27" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B28">
-        <v>220242638</v>
+        <v>220212622</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D28" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" t="s">
-        <v>46</v>
-      </c>
-      <c r="F28" t="s">
-        <v>46</v>
-      </c>
-      <c r="G28" t="s">
-        <v>46</v>
-      </c>
-      <c r="H28" t="s">
-        <v>46</v>
-      </c>
-      <c r="I28" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B29">
-        <v>220253432</v>
+        <v>220224633</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="E29" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B30">
-        <v>220262361</v>
+        <v>220237051</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="D30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" t="s">
+        <v>49</v>
+      </c>
+      <c r="H30" t="s">
+        <v>49</v>
+      </c>
+      <c r="I30" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B31">
-        <v>220264723</v>
+        <v>220242638</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" t="s">
+        <v>49</v>
+      </c>
+      <c r="H31" t="s">
+        <v>49</v>
+      </c>
+      <c r="I31" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B32">
-        <v>220267485</v>
+        <v>220253432</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>38</v>
@@ -1180,10 +1213,10 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33">
-        <v>220289508</v>
+        <v>220262361</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>39</v>
@@ -1191,24 +1224,21 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B34">
-        <v>220289570</v>
+        <v>220264723</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E34" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B35">
-        <v>220294868</v>
+        <v>220267485</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>41</v>
@@ -1216,82 +1246,118 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B36">
-        <v>220322510</v>
+        <v>220289508</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D36" t="s">
-        <v>46</v>
-      </c>
-      <c r="E36" t="s">
-        <v>46</v>
-      </c>
-      <c r="F36" t="s">
-        <v>46</v>
-      </c>
-      <c r="G36" t="s">
-        <v>46</v>
-      </c>
-      <c r="H36" t="s">
-        <v>46</v>
-      </c>
-      <c r="I36" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B37">
-        <v>220327554</v>
+        <v>220289570</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E37" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B38">
-        <v>220377557</v>
+        <v>220294868</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D38" t="s">
-        <v>46</v>
-      </c>
-      <c r="E38" t="s">
-        <v>46</v>
-      </c>
-      <c r="F38" t="s">
-        <v>46</v>
-      </c>
-      <c r="G38" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B39">
-        <v>220494670</v>
+        <v>220322510</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="D39" t="s">
+        <v>49</v>
+      </c>
       <c r="E39" t="s">
+        <v>49</v>
+      </c>
+      <c r="F39" t="s">
+        <v>49</v>
+      </c>
+      <c r="G39" t="s">
+        <v>49</v>
+      </c>
+      <c r="H39" t="s">
+        <v>49</v>
+      </c>
+      <c r="I39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="1">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>220327554</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>46</v>
+      </c>
+      <c r="E40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="1">
+        <v>23</v>
+      </c>
+      <c r="B41">
+        <v>220377557</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" t="s">
+        <v>49</v>
+      </c>
+      <c r="F41" t="s">
+        <v>49</v>
+      </c>
+      <c r="G41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="1">
+        <v>32</v>
+      </c>
+      <c r="B42">
+        <v>220494670</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E42" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1334,6 +1400,9 @@
     <hyperlink ref="C37" r:id="rId36"/>
     <hyperlink ref="C38" r:id="rId37"/>
     <hyperlink ref="C39" r:id="rId38"/>
+    <hyperlink ref="C40" r:id="rId39"/>
+    <hyperlink ref="C41" r:id="rId40"/>
+    <hyperlink ref="C42" r:id="rId41"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1341,7 +1410,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE39"/>
+  <dimension ref="A1:BE42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1355,55 +1424,55 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>5</v>
@@ -1412,109 +1481,109 @@
         <v>4</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="AR1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:57">
@@ -1561,154 +1630,154 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="K5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="M5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="N5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="O5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="Q5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="R5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="S5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="T5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="U5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="V5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="W5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="X5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="Y5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="Z5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AA5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AB5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AC5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AD5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AE5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AF5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AG5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AH5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AI5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AJ5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AK5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AL5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AM5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AO5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AP5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AQ5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AR5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AS5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AU5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AV5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AW5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AX5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AY5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AZ5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="BA5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="BB5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="BC5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="BD5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="BE5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:57">
@@ -1722,49 +1791,49 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="M6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="N6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="Q6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="U6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="V6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="Y6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AA6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AD6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AO6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AR6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AS6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AZ6" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:57">
@@ -1778,25 +1847,25 @@
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="U7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="V7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="Y7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AA7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AR7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AT7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:57">
@@ -1812,156 +1881,198 @@
     </row>
     <row r="9" spans="1:57">
       <c r="A9" s="1">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B9">
-        <v>220019902</v>
+        <v>220018014</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="F9" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>49</v>
+      </c>
+      <c r="R9" t="s">
+        <v>49</v>
+      </c>
+      <c r="S9" t="s">
+        <v>49</v>
+      </c>
+      <c r="U9" t="s">
+        <v>49</v>
+      </c>
+      <c r="V9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10" spans="1:57">
       <c r="A10" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B10">
-        <v>220046953</v>
+        <v>220019902</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U10" t="s">
-        <v>46</v>
-      </c>
-      <c r="V10" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="11" spans="1:57">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B11">
-        <v>220066903</v>
+        <v>220046953</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AT11" t="s">
-        <v>46</v>
+      <c r="U11" t="s">
+        <v>49</v>
+      </c>
+      <c r="V11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:57">
       <c r="A12" s="1">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B12">
-        <v>220068459</v>
+        <v>220055950</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="AT12" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="13" spans="1:57">
       <c r="A13" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B13">
-        <v>220070191</v>
+        <v>220066903</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="AA13" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT13" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="14" spans="1:57">
       <c r="A14" s="1">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B14">
-        <v>220072750</v>
+        <v>220068459</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U14" t="s">
-        <v>46</v>
-      </c>
-      <c r="V14" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>46</v>
-      </c>
-      <c r="AT14" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="15" spans="1:57">
       <c r="A15" s="1">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="B15">
-        <v>220073549</v>
+        <v>220070191</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AT15" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="16" spans="1:57">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B16">
-        <v>220093930</v>
+        <v>220072750</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="U16" t="s">
+        <v>49</v>
+      </c>
+      <c r="V16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT16" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="17" spans="1:52">
       <c r="A17" s="1">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B17">
-        <v>220106745</v>
+        <v>220073549</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="AT17" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="18" spans="1:52">
       <c r="A18" s="1">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B18">
-        <v>220110802</v>
+        <v>220086336</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="U18" t="s">
-        <v>46</v>
-      </c>
-      <c r="V18" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="19" spans="1:52">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19">
-        <v>220126676</v>
+        <v>220093930</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>25</v>
@@ -1969,10 +2080,10 @@
     </row>
     <row r="20" spans="1:52">
       <c r="A20" s="1">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B20">
-        <v>220131060</v>
+        <v>220106745</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>26</v>
@@ -1980,21 +2091,30 @@
     </row>
     <row r="21" spans="1:52">
       <c r="A21" s="1">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B21">
-        <v>220131698</v>
+        <v>220110802</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="U21" t="s">
+        <v>49</v>
+      </c>
+      <c r="V21" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="22" spans="1:52">
       <c r="A22" s="1">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B22">
-        <v>220133606</v>
+        <v>220126676</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>28</v>
@@ -2002,44 +2122,35 @@
     </row>
     <row r="23" spans="1:52">
       <c r="A23" s="1">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>220133692</v>
+        <v>220131060</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="AT23" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="24" spans="1:52">
       <c r="A24" s="1">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B24">
-        <v>220145273</v>
+        <v>220131698</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F24" t="s">
-        <v>46</v>
-      </c>
-      <c r="V24" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="25" spans="1:52">
       <c r="A25" s="1">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B25">
-        <v>220212622</v>
+        <v>220133606</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>31</v>
@@ -2047,163 +2158,178 @@
     </row>
     <row r="26" spans="1:52">
       <c r="A26" s="1">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B26">
-        <v>220224633</v>
+        <v>220133692</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q26" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="27" spans="1:52">
       <c r="A27" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B27">
-        <v>220237051</v>
+        <v>220145273</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F27" t="s">
-        <v>46</v>
-      </c>
-      <c r="I27" t="s">
-        <v>46</v>
-      </c>
-      <c r="J27" t="s">
-        <v>46</v>
-      </c>
-      <c r="L27" t="s">
-        <v>46</v>
-      </c>
-      <c r="M27" t="s">
-        <v>46</v>
-      </c>
-      <c r="N27" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>46</v>
-      </c>
-      <c r="R27" t="s">
-        <v>46</v>
-      </c>
-      <c r="S27" t="s">
-        <v>46</v>
-      </c>
-      <c r="U27" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="V27" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="Y27" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AA27" t="s">
-        <v>46</v>
-      </c>
-      <c r="AN27" t="s">
-        <v>46</v>
-      </c>
-      <c r="AO27" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AR27" t="s">
-        <v>46</v>
-      </c>
-      <c r="AS27" t="s">
-        <v>46</v>
-      </c>
-      <c r="AT27" t="s">
-        <v>46</v>
-      </c>
-      <c r="AX27" t="s">
-        <v>46</v>
-      </c>
-      <c r="AZ27" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:52">
       <c r="A28" s="1">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B28">
-        <v>220242638</v>
+        <v>220212622</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F28" t="s">
-        <v>46</v>
-      </c>
-      <c r="U28" t="s">
-        <v>46</v>
-      </c>
-      <c r="V28" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>46</v>
-      </c>
-      <c r="AR28" t="s">
-        <v>46</v>
-      </c>
-      <c r="AT28" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="29" spans="1:52">
       <c r="A29" s="1">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B29">
-        <v>220253432</v>
+        <v>220224633</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="Q29" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="30" spans="1:52">
       <c r="A30" s="1">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B30">
-        <v>220262361</v>
+        <v>220237051</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="F30" t="s">
+        <v>49</v>
+      </c>
+      <c r="I30" t="s">
+        <v>49</v>
+      </c>
+      <c r="J30" t="s">
+        <v>49</v>
+      </c>
+      <c r="L30" t="s">
+        <v>49</v>
+      </c>
+      <c r="M30" t="s">
+        <v>49</v>
+      </c>
+      <c r="N30" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>49</v>
+      </c>
+      <c r="R30" t="s">
+        <v>49</v>
+      </c>
+      <c r="S30" t="s">
+        <v>49</v>
+      </c>
+      <c r="U30" t="s">
+        <v>49</v>
+      </c>
+      <c r="V30" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN30" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO30" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR30" t="s">
+        <v>49</v>
+      </c>
+      <c r="AS30" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT30" t="s">
+        <v>49</v>
+      </c>
+      <c r="AX30" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ30" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="31" spans="1:52">
       <c r="A31" s="1">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B31">
-        <v>220264723</v>
+        <v>220242638</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="F31" t="s">
+        <v>49</v>
+      </c>
+      <c r="U31" t="s">
+        <v>49</v>
+      </c>
+      <c r="V31" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR31" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT31" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="32" spans="1:52">
       <c r="A32" s="1">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B32">
-        <v>220267485</v>
+        <v>220253432</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>38</v>
@@ -2211,10 +2337,10 @@
     </row>
     <row r="33" spans="1:46">
       <c r="A33" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33">
-        <v>220289508</v>
+        <v>220262361</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>39</v>
@@ -2222,24 +2348,21 @@
     </row>
     <row r="34" spans="1:46">
       <c r="A34" s="1">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B34">
-        <v>220289570</v>
+        <v>220264723</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AA34" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="35" spans="1:46">
       <c r="A35" s="1">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B35">
-        <v>220294868</v>
+        <v>220267485</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>41</v>
@@ -2247,88 +2370,124 @@
     </row>
     <row r="36" spans="1:46">
       <c r="A36" s="1">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B36">
-        <v>220322510</v>
+        <v>220289508</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F36" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>46</v>
-      </c>
-      <c r="U36" t="s">
-        <v>46</v>
-      </c>
-      <c r="V36" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y36" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA36" t="s">
-        <v>46</v>
-      </c>
-      <c r="AR36" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="37" spans="1:46">
       <c r="A37" s="1">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B37">
-        <v>220327554</v>
+        <v>220289570</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>43</v>
       </c>
       <c r="AA37" t="s">
-        <v>46</v>
-      </c>
-      <c r="AT37" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:46">
       <c r="A38" s="1">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B38">
-        <v>220377557</v>
+        <v>220294868</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="U38" t="s">
-        <v>46</v>
-      </c>
-      <c r="V38" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y38" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA38" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="39" spans="1:46">
       <c r="A39" s="1">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B39">
-        <v>220494670</v>
+        <v>220322510</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="F39" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>49</v>
+      </c>
+      <c r="U39" t="s">
+        <v>49</v>
+      </c>
+      <c r="V39" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>49</v>
+      </c>
       <c r="AA39" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:46">
+      <c r="A40" s="1">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>220327554</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>46</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:46">
+      <c r="A41" s="1">
+        <v>23</v>
+      </c>
+      <c r="B41">
+        <v>220377557</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U41" t="s">
+        <v>49</v>
+      </c>
+      <c r="V41" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:46">
+      <c r="A42" s="1">
+        <v>32</v>
+      </c>
+      <c r="B42">
+        <v>220494670</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -2371,6 +2530,9 @@
     <hyperlink ref="C37" r:id="rId36"/>
     <hyperlink ref="C38" r:id="rId37"/>
     <hyperlink ref="C39" r:id="rId38"/>
+    <hyperlink ref="C40" r:id="rId39"/>
+    <hyperlink ref="C41" r:id="rId40"/>
+    <hyperlink ref="C42" r:id="rId41"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2378,7 +2540,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2540,52 +2702,70 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B9">
-        <v>220019902</v>
+        <v>220018014</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D9" s="3">
+        <v>45153</v>
+      </c>
+      <c r="E9" s="3">
+        <v>45148</v>
+      </c>
+      <c r="F9" s="3">
+        <v>45149</v>
+      </c>
+      <c r="G9" s="3">
+        <v>45151</v>
+      </c>
+      <c r="H9" s="3">
+        <v>45155</v>
+      </c>
+      <c r="I9" s="3">
+        <v>45155</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B10">
-        <v>220046953</v>
+        <v>220019902</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="3">
-        <v>45138</v>
-      </c>
-      <c r="F10" s="3">
-        <v>45145</v>
-      </c>
-      <c r="G10" s="3">
-        <v>45154</v>
-      </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B11">
-        <v>220066903</v>
+        <v>220046953</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="E11" s="3">
+        <v>45138</v>
+      </c>
+      <c r="F11" s="3">
+        <v>45145</v>
+      </c>
+      <c r="G11" s="3">
+        <v>45154</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B12">
-        <v>220068459</v>
+        <v>220055950</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>18</v>
@@ -2593,41 +2773,35 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B13">
-        <v>220070191</v>
+        <v>220066903</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="E13" s="3">
+        <v>45158</v>
+      </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B14">
-        <v>220072750</v>
+        <v>220068459</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="3">
-        <v>45154</v>
-      </c>
-      <c r="F14" s="3">
-        <v>45154</v>
-      </c>
-      <c r="G14" s="3">
-        <v>45156</v>
-      </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="B15">
-        <v>220073549</v>
+        <v>220070191</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>21</v>
@@ -2635,21 +2809,30 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B16">
-        <v>220093930</v>
+        <v>220072750</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="E16" s="3">
+        <v>45154</v>
+      </c>
+      <c r="F16" s="3">
+        <v>45154</v>
+      </c>
+      <c r="G16" s="3">
+        <v>45156</v>
+      </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B17">
-        <v>220106745</v>
+        <v>220073549</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>23</v>
@@ -2657,30 +2840,21 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B18">
-        <v>220110802</v>
+        <v>220086336</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="3">
-        <v>45154</v>
-      </c>
-      <c r="F18" s="3">
-        <v>45155</v>
-      </c>
-      <c r="G18" s="3">
-        <v>45155</v>
-      </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19">
-        <v>220126676</v>
+        <v>220093930</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>25</v>
@@ -2688,10 +2862,10 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B20">
-        <v>220131060</v>
+        <v>220106745</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>26</v>
@@ -2699,21 +2873,30 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B21">
-        <v>220131698</v>
+        <v>220110802</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="E21" s="3">
+        <v>45154</v>
+      </c>
+      <c r="F21" s="3">
+        <v>45155</v>
+      </c>
+      <c r="G21" s="3">
+        <v>45155</v>
+      </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B22">
-        <v>220133606</v>
+        <v>220126676</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>28</v>
@@ -2721,10 +2904,10 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>220133692</v>
+        <v>220131060</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>29</v>
@@ -2732,33 +2915,21 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B24">
-        <v>220145273</v>
+        <v>220131698</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="3">
-        <v>45147</v>
-      </c>
-      <c r="E24" s="3">
-        <v>45154</v>
-      </c>
-      <c r="F24" s="3">
-        <v>45155</v>
-      </c>
-      <c r="I24" s="3">
-        <v>45156</v>
-      </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B25">
-        <v>220212622</v>
+        <v>220133606</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>31</v>
@@ -2766,115 +2937,130 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B26">
-        <v>220224633</v>
+        <v>220133692</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="3">
-        <v>44911</v>
-      </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B27">
-        <v>220237051</v>
+        <v>220145273</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D27" s="3">
-        <v>44941</v>
+        <v>45147</v>
       </c>
       <c r="E27" s="3">
-        <v>44939</v>
+        <v>45154</v>
       </c>
       <c r="F27" s="3">
-        <v>44939</v>
-      </c>
-      <c r="G27" s="3">
-        <v>44940</v>
+        <v>45155</v>
       </c>
       <c r="H27" s="3">
-        <v>44951</v>
+        <v>45158</v>
       </c>
       <c r="I27" s="3">
-        <v>44952</v>
+        <v>45156</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B28">
-        <v>220242638</v>
+        <v>220212622</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="3">
-        <v>45156</v>
-      </c>
-      <c r="E28" s="3">
-        <v>45151</v>
-      </c>
-      <c r="F28" s="3">
-        <v>45155</v>
-      </c>
-      <c r="G28" s="3">
-        <v>45155</v>
-      </c>
-      <c r="H28" s="3">
-        <v>45157</v>
-      </c>
-      <c r="I28" s="3">
-        <v>45157</v>
-      </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B29">
-        <v>220253432</v>
+        <v>220224633</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="E29" s="3">
+        <v>44911</v>
+      </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B30">
-        <v>220262361</v>
+        <v>220237051</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="D30" s="3">
+        <v>44941</v>
+      </c>
+      <c r="E30" s="3">
+        <v>44939</v>
+      </c>
+      <c r="F30" s="3">
+        <v>44939</v>
+      </c>
+      <c r="G30" s="3">
+        <v>44940</v>
+      </c>
+      <c r="H30" s="3">
+        <v>44951</v>
+      </c>
+      <c r="I30" s="3">
+        <v>44952</v>
+      </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B31">
-        <v>220264723</v>
+        <v>220242638</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="D31" s="3">
+        <v>45156</v>
+      </c>
+      <c r="E31" s="3">
+        <v>45151</v>
+      </c>
+      <c r="F31" s="3">
+        <v>45155</v>
+      </c>
+      <c r="G31" s="3">
+        <v>45155</v>
+      </c>
+      <c r="H31" s="3">
+        <v>45157</v>
+      </c>
+      <c r="I31" s="3">
+        <v>45157</v>
+      </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B32">
-        <v>220267485</v>
+        <v>220253432</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>38</v>
@@ -2882,10 +3068,10 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33">
-        <v>220289508</v>
+        <v>220262361</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>39</v>
@@ -2893,24 +3079,21 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B34">
-        <v>220289570</v>
+        <v>220264723</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E34" s="3">
-        <v>45156</v>
-      </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B35">
-        <v>220294868</v>
+        <v>220267485</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>41</v>
@@ -2918,81 +3101,117 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B36">
-        <v>220322510</v>
+        <v>220289508</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="3">
-        <v>45149</v>
-      </c>
-      <c r="E36" s="3">
-        <v>45145</v>
-      </c>
-      <c r="F36" s="3">
-        <v>45146</v>
-      </c>
-      <c r="G36" s="3">
-        <v>45147</v>
-      </c>
-      <c r="H36" s="3">
-        <v>45150</v>
-      </c>
-      <c r="I36" s="3">
-        <v>45151</v>
-      </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B37">
-        <v>220327554</v>
+        <v>220289570</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E37" s="3">
-        <v>45157</v>
+        <v>45156</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B38">
-        <v>220377557</v>
+        <v>220294868</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="3">
-        <v>45149</v>
-      </c>
-      <c r="E38" s="3">
-        <v>45154</v>
-      </c>
-      <c r="F38" s="3">
-        <v>45158</v>
-      </c>
-      <c r="G38" s="3">
-        <v>45158</v>
-      </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B39">
-        <v>220494670</v>
+        <v>220322510</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="D39" s="3">
+        <v>45149</v>
+      </c>
       <c r="E39" s="3">
+        <v>45145</v>
+      </c>
+      <c r="F39" s="3">
+        <v>45146</v>
+      </c>
+      <c r="G39" s="3">
+        <v>45147</v>
+      </c>
+      <c r="H39" s="3">
+        <v>45150</v>
+      </c>
+      <c r="I39" s="3">
+        <v>45151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="1">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>220327554</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E40" s="3">
+        <v>45157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="1">
+        <v>23</v>
+      </c>
+      <c r="B41">
+        <v>220377557</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="3">
+        <v>45149</v>
+      </c>
+      <c r="E41" s="3">
+        <v>45154</v>
+      </c>
+      <c r="F41" s="3">
+        <v>45158</v>
+      </c>
+      <c r="G41" s="3">
+        <v>45158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="1">
+        <v>32</v>
+      </c>
+      <c r="B42">
+        <v>220494670</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E42" s="3">
         <v>45157</v>
       </c>
     </row>
@@ -3036,6 +3255,9 @@
     <hyperlink ref="C37" r:id="rId36"/>
     <hyperlink ref="C38" r:id="rId37"/>
     <hyperlink ref="C39" r:id="rId38"/>
+    <hyperlink ref="C40" r:id="rId39"/>
+    <hyperlink ref="C41" r:id="rId40"/>
+    <hyperlink ref="C42" r:id="rId41"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3043,7 +3265,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BE39"/>
+  <dimension ref="A1:BE42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3057,55 +3279,55 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>5</v>
@@ -3114,109 +3336,109 @@
         <v>4</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="AR1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:57">
@@ -3514,156 +3736,198 @@
     </row>
     <row r="9" spans="1:57">
       <c r="A9" s="1">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B9">
-        <v>220019902</v>
+        <v>220018014</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="F9" s="3">
+        <v>45155</v>
+      </c>
+      <c r="I9" s="3">
+        <v>45156</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>45154</v>
+      </c>
+      <c r="R9" s="3">
+        <v>45156</v>
+      </c>
+      <c r="S9" s="3">
+        <v>45152</v>
+      </c>
+      <c r="U9" s="3">
+        <v>45151</v>
+      </c>
+      <c r="V9" s="3">
+        <v>45149</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>45153</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>45148</v>
+      </c>
+      <c r="AN9" s="3">
+        <v>45153</v>
+      </c>
+      <c r="AR9" s="3">
+        <v>45155</v>
+      </c>
+      <c r="AS9" s="3">
+        <v>45154</v>
+      </c>
+      <c r="AT9" s="3">
+        <v>45148</v>
+      </c>
+      <c r="AX9" s="3">
+        <v>45153</v>
+      </c>
+      <c r="AZ9" s="3">
+        <v>45154</v>
+      </c>
     </row>
     <row r="10" spans="1:57">
       <c r="A10" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B10">
-        <v>220046953</v>
+        <v>220019902</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U10" s="3">
-        <v>45154</v>
-      </c>
-      <c r="V10" s="3">
-        <v>45145</v>
-      </c>
-      <c r="AA10" s="3">
-        <v>45138</v>
-      </c>
     </row>
     <row r="11" spans="1:57">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B11">
-        <v>220066903</v>
+        <v>220046953</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AT11" s="3">
-        <v>45152</v>
+      <c r="U11" s="3">
+        <v>45154</v>
+      </c>
+      <c r="V11" s="3">
+        <v>45145</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>45138</v>
       </c>
     </row>
     <row r="12" spans="1:57">
       <c r="A12" s="1">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B12">
-        <v>220068459</v>
+        <v>220055950</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="AT12" s="3">
+        <v>45158</v>
+      </c>
     </row>
     <row r="13" spans="1:57">
       <c r="A13" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B13">
-        <v>220070191</v>
+        <v>220066903</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="AA13" s="3">
+        <v>45158</v>
+      </c>
+      <c r="AT13" s="3">
+        <v>45152</v>
+      </c>
     </row>
     <row r="14" spans="1:57">
       <c r="A14" s="1">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B14">
-        <v>220072750</v>
+        <v>220068459</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U14" s="3">
-        <v>45156</v>
-      </c>
-      <c r="V14" s="3">
-        <v>45154</v>
-      </c>
-      <c r="AA14" s="3">
-        <v>45154</v>
-      </c>
-      <c r="AT14" s="3">
-        <v>45153</v>
-      </c>
     </row>
     <row r="15" spans="1:57">
       <c r="A15" s="1">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="B15">
-        <v>220073549</v>
+        <v>220070191</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AT15" s="3">
-        <v>45145</v>
-      </c>
     </row>
     <row r="16" spans="1:57">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B16">
-        <v>220093930</v>
+        <v>220072750</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="U16" s="3">
+        <v>45156</v>
+      </c>
+      <c r="V16" s="3">
+        <v>45154</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>45154</v>
+      </c>
+      <c r="AT16" s="3">
+        <v>45153</v>
+      </c>
     </row>
     <row r="17" spans="1:52">
       <c r="A17" s="1">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B17">
-        <v>220106745</v>
+        <v>220073549</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="AT17" s="3">
+        <v>45145</v>
+      </c>
     </row>
     <row r="18" spans="1:52">
       <c r="A18" s="1">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B18">
-        <v>220110802</v>
+        <v>220086336</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="U18" s="3">
-        <v>45155</v>
-      </c>
-      <c r="V18" s="3">
-        <v>45155</v>
-      </c>
-      <c r="AA18" s="3">
-        <v>45154</v>
-      </c>
     </row>
     <row r="19" spans="1:52">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19">
-        <v>220126676</v>
+        <v>220093930</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>25</v>
@@ -3671,10 +3935,10 @@
     </row>
     <row r="20" spans="1:52">
       <c r="A20" s="1">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B20">
-        <v>220131060</v>
+        <v>220106745</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>26</v>
@@ -3682,21 +3946,30 @@
     </row>
     <row r="21" spans="1:52">
       <c r="A21" s="1">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B21">
-        <v>220131698</v>
+        <v>220110802</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="U21" s="3">
+        <v>45155</v>
+      </c>
+      <c r="V21" s="3">
+        <v>45155</v>
+      </c>
+      <c r="AA21" s="3">
+        <v>45154</v>
+      </c>
     </row>
     <row r="22" spans="1:52">
       <c r="A22" s="1">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="B22">
-        <v>220133606</v>
+        <v>220126676</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>28</v>
@@ -3704,44 +3977,35 @@
     </row>
     <row r="23" spans="1:52">
       <c r="A23" s="1">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B23">
-        <v>220133692</v>
+        <v>220131060</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="AT23" s="3">
+        <v>45158</v>
+      </c>
     </row>
     <row r="24" spans="1:52">
       <c r="A24" s="1">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B24">
-        <v>220145273</v>
+        <v>220131698</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F24" s="3">
-        <v>45156</v>
-      </c>
-      <c r="V24" s="3">
-        <v>45155</v>
-      </c>
-      <c r="Y24" s="3">
-        <v>45147</v>
-      </c>
-      <c r="AA24" s="3">
-        <v>45154</v>
-      </c>
     </row>
     <row r="25" spans="1:52">
       <c r="A25" s="1">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B25">
-        <v>220212622</v>
+        <v>220133606</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>31</v>
@@ -3749,163 +4013,178 @@
     </row>
     <row r="26" spans="1:52">
       <c r="A26" s="1">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B26">
-        <v>220224633</v>
+        <v>220133692</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q26" s="3">
-        <v>44852</v>
-      </c>
-      <c r="AA26" s="3">
-        <v>44911</v>
-      </c>
     </row>
     <row r="27" spans="1:52">
       <c r="A27" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B27">
-        <v>220237051</v>
+        <v>220145273</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F27" s="3">
-        <v>44952</v>
-      </c>
-      <c r="I27" s="3">
-        <v>44951</v>
-      </c>
-      <c r="J27" s="3">
-        <v>44943</v>
-      </c>
-      <c r="L27" s="3">
-        <v>45015</v>
-      </c>
-      <c r="M27" s="3">
-        <v>45014</v>
-      </c>
-      <c r="N27" s="3">
-        <v>45014</v>
-      </c>
-      <c r="Q27" s="3">
-        <v>44846</v>
-      </c>
-      <c r="R27" s="3">
-        <v>44951</v>
-      </c>
-      <c r="S27" s="3">
-        <v>44940</v>
-      </c>
-      <c r="U27" s="3">
-        <v>44940</v>
+        <v>45156</v>
       </c>
       <c r="V27" s="3">
-        <v>44939</v>
+        <v>45155</v>
       </c>
       <c r="Y27" s="3">
-        <v>44941</v>
+        <v>45147</v>
       </c>
       <c r="AA27" s="3">
-        <v>44939</v>
-      </c>
-      <c r="AN27" s="3">
-        <v>44942</v>
-      </c>
-      <c r="AO27" s="3">
-        <v>45015</v>
+        <v>45154</v>
       </c>
       <c r="AR27" s="3">
-        <v>44951</v>
-      </c>
-      <c r="AS27" s="3">
-        <v>44939</v>
-      </c>
-      <c r="AT27" s="3">
-        <v>44936</v>
-      </c>
-      <c r="AX27" s="3">
-        <v>44941</v>
-      </c>
-      <c r="AZ27" s="3">
-        <v>44948</v>
+        <v>45158</v>
       </c>
     </row>
     <row r="28" spans="1:52">
       <c r="A28" s="1">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B28">
-        <v>220242638</v>
+        <v>220212622</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="3">
-        <v>45157</v>
-      </c>
-      <c r="U28" s="3">
-        <v>45155</v>
-      </c>
-      <c r="V28" s="3">
-        <v>45155</v>
-      </c>
-      <c r="Y28" s="3">
-        <v>45156</v>
-      </c>
-      <c r="AA28" s="3">
-        <v>45151</v>
-      </c>
-      <c r="AR28" s="3">
-        <v>45157</v>
-      </c>
-      <c r="AT28" s="3">
-        <v>45150</v>
-      </c>
     </row>
     <row r="29" spans="1:52">
       <c r="A29" s="1">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B29">
-        <v>220253432</v>
+        <v>220224633</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="Q29" s="3">
+        <v>44852</v>
+      </c>
+      <c r="AA29" s="3">
+        <v>44911</v>
+      </c>
     </row>
     <row r="30" spans="1:52">
       <c r="A30" s="1">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B30">
-        <v>220262361</v>
+        <v>220237051</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="F30" s="3">
+        <v>44952</v>
+      </c>
+      <c r="I30" s="3">
+        <v>44951</v>
+      </c>
+      <c r="J30" s="3">
+        <v>44943</v>
+      </c>
+      <c r="L30" s="3">
+        <v>45015</v>
+      </c>
+      <c r="M30" s="3">
+        <v>45014</v>
+      </c>
+      <c r="N30" s="3">
+        <v>45014</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>44846</v>
+      </c>
+      <c r="R30" s="3">
+        <v>44951</v>
+      </c>
+      <c r="S30" s="3">
+        <v>44940</v>
+      </c>
+      <c r="U30" s="3">
+        <v>44940</v>
+      </c>
+      <c r="V30" s="3">
+        <v>44939</v>
+      </c>
+      <c r="Y30" s="3">
+        <v>44941</v>
+      </c>
+      <c r="AA30" s="3">
+        <v>44939</v>
+      </c>
+      <c r="AN30" s="3">
+        <v>44942</v>
+      </c>
+      <c r="AO30" s="3">
+        <v>45015</v>
+      </c>
+      <c r="AR30" s="3">
+        <v>44951</v>
+      </c>
+      <c r="AS30" s="3">
+        <v>44939</v>
+      </c>
+      <c r="AT30" s="3">
+        <v>44936</v>
+      </c>
+      <c r="AX30" s="3">
+        <v>44941</v>
+      </c>
+      <c r="AZ30" s="3">
+        <v>44948</v>
+      </c>
     </row>
     <row r="31" spans="1:52">
       <c r="A31" s="1">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B31">
-        <v>220264723</v>
+        <v>220242638</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="F31" s="3">
+        <v>45157</v>
+      </c>
+      <c r="U31" s="3">
+        <v>45155</v>
+      </c>
+      <c r="V31" s="3">
+        <v>45155</v>
+      </c>
+      <c r="Y31" s="3">
+        <v>45156</v>
+      </c>
+      <c r="AA31" s="3">
+        <v>45151</v>
+      </c>
+      <c r="AR31" s="3">
+        <v>45157</v>
+      </c>
+      <c r="AT31" s="3">
+        <v>45150</v>
+      </c>
     </row>
     <row r="32" spans="1:52">
       <c r="A32" s="1">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B32">
-        <v>220267485</v>
+        <v>220253432</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>38</v>
@@ -3913,10 +4192,10 @@
     </row>
     <row r="33" spans="1:46">
       <c r="A33" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33">
-        <v>220289508</v>
+        <v>220262361</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>39</v>
@@ -3924,24 +4203,21 @@
     </row>
     <row r="34" spans="1:46">
       <c r="A34" s="1">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B34">
-        <v>220289570</v>
+        <v>220264723</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AA34" s="3">
-        <v>45156</v>
-      </c>
     </row>
     <row r="35" spans="1:46">
       <c r="A35" s="1">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B35">
-        <v>220294868</v>
+        <v>220267485</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>41</v>
@@ -3949,87 +4225,123 @@
     </row>
     <row r="36" spans="1:46">
       <c r="A36" s="1">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B36">
-        <v>220322510</v>
+        <v>220289508</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F36" s="3">
-        <v>45151</v>
-      </c>
-      <c r="Q36" s="3">
-        <v>45155</v>
-      </c>
-      <c r="U36" s="3">
-        <v>45147</v>
-      </c>
-      <c r="V36" s="3">
-        <v>45146</v>
-      </c>
-      <c r="Y36" s="3">
-        <v>45149</v>
-      </c>
-      <c r="AA36" s="3">
-        <v>45145</v>
-      </c>
-      <c r="AR36" s="3">
-        <v>45150</v>
-      </c>
     </row>
     <row r="37" spans="1:46">
       <c r="A37" s="1">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B37">
-        <v>220327554</v>
+        <v>220289570</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>43</v>
       </c>
       <c r="AA37" s="3">
-        <v>45157</v>
-      </c>
-      <c r="AT37" s="3">
-        <v>45152</v>
+        <v>45156</v>
       </c>
     </row>
     <row r="38" spans="1:46">
       <c r="A38" s="1">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B38">
-        <v>220377557</v>
+        <v>220294868</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="U38" s="3">
-        <v>45158</v>
-      </c>
-      <c r="V38" s="3">
-        <v>45158</v>
-      </c>
-      <c r="Y38" s="3">
-        <v>45149</v>
-      </c>
-      <c r="AA38" s="3">
-        <v>45154</v>
-      </c>
     </row>
     <row r="39" spans="1:46">
       <c r="A39" s="1">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="B39">
-        <v>220494670</v>
+        <v>220322510</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="F39" s="3">
+        <v>45151</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>45155</v>
+      </c>
+      <c r="U39" s="3">
+        <v>45147</v>
+      </c>
+      <c r="V39" s="3">
+        <v>45146</v>
+      </c>
+      <c r="Y39" s="3">
+        <v>45149</v>
+      </c>
       <c r="AA39" s="3">
+        <v>45145</v>
+      </c>
+      <c r="AR39" s="3">
+        <v>45150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:46">
+      <c r="A40" s="1">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>220327554</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA40" s="3">
+        <v>45157</v>
+      </c>
+      <c r="AT40" s="3">
+        <v>45152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:46">
+      <c r="A41" s="1">
+        <v>23</v>
+      </c>
+      <c r="B41">
+        <v>220377557</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U41" s="3">
+        <v>45158</v>
+      </c>
+      <c r="V41" s="3">
+        <v>45158</v>
+      </c>
+      <c r="Y41" s="3">
+        <v>45149</v>
+      </c>
+      <c r="AA41" s="3">
+        <v>45154</v>
+      </c>
+    </row>
+    <row r="42" spans="1:46">
+      <c r="A42" s="1">
+        <v>32</v>
+      </c>
+      <c r="B42">
+        <v>220494670</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA42" s="3">
         <v>45157</v>
       </c>
     </row>
@@ -4073,6 +4385,9 @@
     <hyperlink ref="C37" r:id="rId36"/>
     <hyperlink ref="C38" r:id="rId37"/>
     <hyperlink ref="C39" r:id="rId38"/>
+    <hyperlink ref="C40" r:id="rId39"/>
+    <hyperlink ref="C41" r:id="rId40"/>
+    <hyperlink ref="C42" r:id="rId41"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Bug fix for the change of CSS.
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="160">
   <si>
     <t>ID</t>
   </si>
@@ -355,6 +355,9 @@
     <t>Exploring Data with Looker</t>
   </si>
   <si>
+    <t>Generative AI Explorer - Vertex AI</t>
+  </si>
+  <si>
     <t>Google Cloud Essentials</t>
   </si>
   <si>
@@ -376,6 +379,12 @@
     <t>Introduction to Generative AI</t>
   </si>
   <si>
+    <t>Introduction to Large Language Models</t>
+  </si>
+  <si>
+    <t>Introduction to Responsible AI</t>
+  </si>
+  <si>
     <t>Kubernetes in Google Cloud</t>
   </si>
   <si>
@@ -385,6 +394,9 @@
     <t>Level 1: BigQuery ML, Cloud Architecture and Devops Skills</t>
   </si>
   <si>
+    <t>Level 1: Data Analysis and Serverless Technologies</t>
+  </si>
+  <si>
     <t>Level 1: Data, ML and API Skills</t>
   </si>
   <si>
@@ -404,6 +416,12 @@
   </si>
   <si>
     <t>Level 2: Data Exploration with Looker, BigQuery and Sheets</t>
+  </si>
+  <si>
+    <t>Level 2: Security and Monitoring</t>
+  </si>
+  <si>
+    <t>Level 3 GenAI: Prompt Engineering</t>
   </si>
   <si>
     <t>Level 3: GenAI</t>
@@ -1291,7 +1309,7 @@
         <v>10</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>25</v>
@@ -1300,6 +1318,9 @@
         <v>88</v>
       </c>
       <c r="G15" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2240,7 +2261,7 @@
         <v>10</v>
       </c>
       <c r="D47">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>57</v>
@@ -2255,6 +2276,9 @@
         <v>88</v>
       </c>
       <c r="I47" t="s">
+        <v>88</v>
+      </c>
+      <c r="K47" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3150,13 +3174,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BV77"/>
+  <dimension ref="A1:CB77"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:74">
+    <row r="1" spans="1:80">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3242,16 +3266,16 @@
         <v>111</v>
       </c>
       <c r="AD1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="AF1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>114</v>
@@ -3317,25 +3341,25 @@
         <v>134</v>
       </c>
       <c r="BC1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="BI1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="BJ1" s="1" t="s">
         <v>141</v>
@@ -3376,8 +3400,26 @@
       <c r="BV1" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="2" spans="1:74">
+      <c r="BW1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:80">
       <c r="A2" s="1">
         <v>79</v>
       </c>
@@ -3388,7 +3430,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:74">
+    <row r="3" spans="1:80">
       <c r="A3" s="1">
         <v>58</v>
       </c>
@@ -3407,17 +3449,17 @@
       <c r="AA3" t="s">
         <v>88</v>
       </c>
-      <c r="AD3" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:74">
+      <c r="AE3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:80">
       <c r="A4" s="1">
         <v>46</v>
       </c>
@@ -3427,14 +3469,14 @@
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:74">
+      <c r="AE4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:80">
       <c r="A5" s="1">
         <v>21</v>
       </c>
@@ -3445,7 +3487,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:74">
+    <row r="6" spans="1:80">
       <c r="A6" s="1">
         <v>12</v>
       </c>
@@ -3456,7 +3498,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:74">
+    <row r="7" spans="1:80">
       <c r="A7" s="1">
         <v>27</v>
       </c>
@@ -3478,20 +3520,20 @@
       <c r="AA7" t="s">
         <v>88</v>
       </c>
-      <c r="AD7" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC7" t="s">
-        <v>88</v>
-      </c>
-      <c r="BE7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:74">
+      <c r="AE7" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI7" t="s">
+        <v>88</v>
+      </c>
+      <c r="BK7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:80">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -3585,7 +3627,7 @@
       <c r="AI8" t="s">
         <v>88</v>
       </c>
-      <c r="AL8" t="s">
+      <c r="AJ8" t="s">
         <v>88</v>
       </c>
       <c r="AM8" t="s">
@@ -3621,27 +3663,30 @@
       <c r="AW8" t="s">
         <v>88</v>
       </c>
+      <c r="AX8" t="s">
+        <v>88</v>
+      </c>
       <c r="AY8" t="s">
         <v>88</v>
       </c>
       <c r="AZ8" t="s">
         <v>88</v>
       </c>
+      <c r="BA8" t="s">
+        <v>88</v>
+      </c>
       <c r="BB8" t="s">
         <v>88</v>
       </c>
       <c r="BC8" t="s">
         <v>88</v>
       </c>
-      <c r="BD8" t="s">
+      <c r="BE8" t="s">
         <v>88</v>
       </c>
       <c r="BF8" t="s">
         <v>88</v>
       </c>
-      <c r="BG8" t="s">
-        <v>88</v>
-      </c>
       <c r="BH8" t="s">
         <v>88</v>
       </c>
@@ -3651,9 +3696,6 @@
       <c r="BJ8" t="s">
         <v>88</v>
       </c>
-      <c r="BK8" t="s">
-        <v>88</v>
-      </c>
       <c r="BL8" t="s">
         <v>88</v>
       </c>
@@ -3687,8 +3729,26 @@
       <c r="BV8" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="9" spans="1:74">
+      <c r="BW8" t="s">
+        <v>88</v>
+      </c>
+      <c r="BX8" t="s">
+        <v>88</v>
+      </c>
+      <c r="BY8" t="s">
+        <v>88</v>
+      </c>
+      <c r="BZ8" t="s">
+        <v>88</v>
+      </c>
+      <c r="CA8" t="s">
+        <v>88</v>
+      </c>
+      <c r="CB8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:80">
       <c r="A9" s="1">
         <v>18</v>
       </c>
@@ -3722,29 +3782,29 @@
       <c r="AA9" t="s">
         <v>88</v>
       </c>
-      <c r="AD9" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>88</v>
-      </c>
-      <c r="AI9" t="s">
-        <v>88</v>
-      </c>
-      <c r="AY9" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC9" t="s">
-        <v>88</v>
-      </c>
-      <c r="BD9" t="s">
-        <v>88</v>
-      </c>
-      <c r="BQ9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:74">
+      <c r="AE9" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>88</v>
+      </c>
+      <c r="BE9" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI9" t="s">
+        <v>88</v>
+      </c>
+      <c r="BJ9" t="s">
+        <v>88</v>
+      </c>
+      <c r="BW9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:80">
       <c r="A10" s="1">
         <v>19</v>
       </c>
@@ -3763,20 +3823,20 @@
       <c r="AA10" t="s">
         <v>88</v>
       </c>
-      <c r="AD10" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC10" t="s">
-        <v>88</v>
-      </c>
-      <c r="BE10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:74">
+      <c r="AE10" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI10" t="s">
+        <v>88</v>
+      </c>
+      <c r="BK10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:80">
       <c r="A11" s="1">
         <v>16</v>
       </c>
@@ -3798,17 +3858,17 @@
       <c r="AA11" t="s">
         <v>88</v>
       </c>
-      <c r="AD11" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:74">
+      <c r="AE11" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:80">
       <c r="A12" s="1">
         <v>40</v>
       </c>
@@ -3839,32 +3899,32 @@
       <c r="AA12" t="s">
         <v>88</v>
       </c>
-      <c r="AD12" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>88</v>
-      </c>
-      <c r="AX12" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC12" t="s">
+      <c r="AE12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG12" t="s">
         <v>88</v>
       </c>
       <c r="BD12" t="s">
         <v>88</v>
       </c>
-      <c r="BE12" t="s">
-        <v>88</v>
-      </c>
-      <c r="BN12" t="s">
-        <v>88</v>
-      </c>
-      <c r="BQ12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:74">
+      <c r="BI12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BJ12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BK12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BT12" t="s">
+        <v>88</v>
+      </c>
+      <c r="BW12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:80">
       <c r="A13" s="1">
         <v>6</v>
       </c>
@@ -3883,17 +3943,17 @@
       <c r="AA13" t="s">
         <v>88</v>
       </c>
-      <c r="AD13" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:74">
+      <c r="AE13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:80">
       <c r="A14" s="1">
         <v>59</v>
       </c>
@@ -3912,17 +3972,17 @@
       <c r="AA14" t="s">
         <v>88</v>
       </c>
-      <c r="AD14" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:74">
+      <c r="AE14" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:80">
       <c r="A15" s="1">
         <v>70</v>
       </c>
@@ -3932,14 +3992,17 @@
       <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AD15" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:74">
+      <c r="AA15" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:80">
       <c r="A16" s="1">
         <v>47</v>
       </c>
@@ -3958,17 +4021,17 @@
       <c r="AA16" t="s">
         <v>88</v>
       </c>
-      <c r="AD16" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF16" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:66">
+      <c r="AE16" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:72">
       <c r="A17" s="1">
         <v>54</v>
       </c>
@@ -3979,7 +4042,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:66">
+    <row r="18" spans="1:72">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -3998,17 +4061,17 @@
       <c r="AA18" t="s">
         <v>88</v>
       </c>
-      <c r="AD18" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF18" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:66">
+      <c r="AE18" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:72">
       <c r="A19" s="1">
         <v>41</v>
       </c>
@@ -4027,17 +4090,17 @@
       <c r="AA19" t="s">
         <v>88</v>
       </c>
-      <c r="AD19" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF19" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC19" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:66">
+      <c r="AE19" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:72">
       <c r="A20" s="1">
         <v>9</v>
       </c>
@@ -4059,20 +4122,20 @@
       <c r="AA20" t="s">
         <v>88</v>
       </c>
-      <c r="AD20" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF20" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC20" t="s">
-        <v>88</v>
-      </c>
-      <c r="BE20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:66">
+      <c r="AE20" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI20" t="s">
+        <v>88</v>
+      </c>
+      <c r="BK20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:72">
       <c r="A21" s="1">
         <v>30</v>
       </c>
@@ -4083,7 +4146,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:66">
+    <row r="22" spans="1:72">
       <c r="A22" s="1">
         <v>4</v>
       </c>
@@ -4102,17 +4165,17 @@
       <c r="AA22" t="s">
         <v>88</v>
       </c>
-      <c r="AD22" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF22" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC22" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:66">
+      <c r="AE22" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:72">
       <c r="A23" s="1">
         <v>64</v>
       </c>
@@ -4123,7 +4186,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:66">
+    <row r="24" spans="1:72">
       <c r="A24" s="1">
         <v>10</v>
       </c>
@@ -4142,20 +4205,20 @@
       <c r="AA24" t="s">
         <v>88</v>
       </c>
-      <c r="AD24" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF24" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC24" t="s">
-        <v>88</v>
-      </c>
-      <c r="BE24" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:66">
+      <c r="AE24" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI24" t="s">
+        <v>88</v>
+      </c>
+      <c r="BK24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:72">
       <c r="A25" s="1">
         <v>33</v>
       </c>
@@ -4174,20 +4237,20 @@
       <c r="AA25" t="s">
         <v>88</v>
       </c>
-      <c r="AD25" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF25" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC25" t="s">
-        <v>88</v>
-      </c>
-      <c r="BE25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:66">
+      <c r="AE25" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG25" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI25" t="s">
+        <v>88</v>
+      </c>
+      <c r="BK25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:72">
       <c r="A26" s="1">
         <v>52</v>
       </c>
@@ -4198,7 +4261,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:66">
+    <row r="27" spans="1:72">
       <c r="A27" s="1">
         <v>62</v>
       </c>
@@ -4217,17 +4280,17 @@
       <c r="AA27" t="s">
         <v>88</v>
       </c>
-      <c r="AD27" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF27" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC27" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:66">
+      <c r="AE27" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:72">
       <c r="A28" s="1">
         <v>69</v>
       </c>
@@ -4238,7 +4301,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:66">
+    <row r="29" spans="1:72">
       <c r="A29" s="1">
         <v>38</v>
       </c>
@@ -4257,17 +4320,17 @@
       <c r="AA29" t="s">
         <v>88</v>
       </c>
-      <c r="AD29" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF29" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC29" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:66">
+      <c r="AE29" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG29" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:72">
       <c r="A30" s="1">
         <v>15</v>
       </c>
@@ -4286,17 +4349,17 @@
       <c r="AA30" t="s">
         <v>88</v>
       </c>
-      <c r="AD30" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF30" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC30" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:66">
+      <c r="AE30" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:72">
       <c r="A31" s="1">
         <v>37</v>
       </c>
@@ -4315,23 +4378,23 @@
       <c r="AA31" t="s">
         <v>88</v>
       </c>
-      <c r="AD31" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF31" t="s">
-        <v>88</v>
-      </c>
-      <c r="AX31" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC31" t="s">
-        <v>88</v>
-      </c>
-      <c r="BN31" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:66">
+      <c r="AE31" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>88</v>
+      </c>
+      <c r="BD31" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI31" t="s">
+        <v>88</v>
+      </c>
+      <c r="BT31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:72">
       <c r="A32" s="1">
         <v>11</v>
       </c>
@@ -4350,17 +4413,17 @@
       <c r="AA32" t="s">
         <v>88</v>
       </c>
-      <c r="AD32" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF32" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:69">
+      <c r="AE32" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG32" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:75">
       <c r="A33" s="1">
         <v>56</v>
       </c>
@@ -4379,17 +4442,17 @@
       <c r="AA33" t="s">
         <v>88</v>
       </c>
-      <c r="AD33" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF33" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC33" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="1:69">
+      <c r="AE33" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:75">
       <c r="A34" s="1">
         <v>17</v>
       </c>
@@ -4408,17 +4471,17 @@
       <c r="AA34" t="s">
         <v>88</v>
       </c>
-      <c r="AD34" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF34" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC34" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:69">
+      <c r="AE34" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG34" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:75">
       <c r="A35" s="1">
         <v>22</v>
       </c>
@@ -4434,20 +4497,20 @@
       <c r="AA35" t="s">
         <v>88</v>
       </c>
-      <c r="AD35" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF35" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC35" t="s">
-        <v>88</v>
-      </c>
-      <c r="BE35" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="36" spans="1:69">
+      <c r="AE35" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG35" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI35" t="s">
+        <v>88</v>
+      </c>
+      <c r="BK35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:75">
       <c r="A36" s="1">
         <v>78</v>
       </c>
@@ -4458,7 +4521,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:69">
+    <row r="37" spans="1:75">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -4477,17 +4540,17 @@
       <c r="AA37" t="s">
         <v>88</v>
       </c>
-      <c r="AD37" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF37" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC37" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="38" spans="1:69">
+      <c r="AE37" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG37" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:75">
       <c r="A38" s="1">
         <v>34</v>
       </c>
@@ -4506,17 +4569,17 @@
       <c r="AA38" t="s">
         <v>88</v>
       </c>
-      <c r="AD38" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF38" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC38" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="39" spans="1:69">
+      <c r="AE38" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG38" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:75">
       <c r="A39" s="1">
         <v>13</v>
       </c>
@@ -4535,17 +4598,17 @@
       <c r="AA39" t="s">
         <v>88</v>
       </c>
-      <c r="AD39" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF39" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC39" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:69">
+      <c r="AE39" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG39" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:75">
       <c r="A40" s="1">
         <v>65</v>
       </c>
@@ -4564,17 +4627,17 @@
       <c r="AA40" t="s">
         <v>88</v>
       </c>
-      <c r="AD40" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF40" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC40" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="41" spans="1:69">
+      <c r="AE40" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG40" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:75">
       <c r="A41" s="1">
         <v>66</v>
       </c>
@@ -4587,14 +4650,14 @@
       <c r="Z41" t="s">
         <v>88</v>
       </c>
-      <c r="AF41" t="s">
-        <v>88</v>
-      </c>
-      <c r="BE41" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="42" spans="1:69">
+      <c r="AG41" t="s">
+        <v>88</v>
+      </c>
+      <c r="BK41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:75">
       <c r="A42" s="1">
         <v>68</v>
       </c>
@@ -4613,17 +4676,17 @@
       <c r="AA42" t="s">
         <v>88</v>
       </c>
-      <c r="AD42" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF42" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC42" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="43" spans="1:69">
+      <c r="AE42" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG42" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:75">
       <c r="A43" s="1">
         <v>8</v>
       </c>
@@ -4642,17 +4705,17 @@
       <c r="AA43" t="s">
         <v>88</v>
       </c>
-      <c r="AD43" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF43" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC43" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" spans="1:69">
+      <c r="AE43" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG43" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:75">
       <c r="A44" s="1">
         <v>60</v>
       </c>
@@ -4671,17 +4734,17 @@
       <c r="AA44" t="s">
         <v>88</v>
       </c>
-      <c r="AD44" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF44" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC44" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="45" spans="1:69">
+      <c r="AE44" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG44" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:75">
       <c r="A45" s="1">
         <v>61</v>
       </c>
@@ -4692,7 +4755,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:69">
+    <row r="46" spans="1:75">
       <c r="A46" s="1">
         <v>63</v>
       </c>
@@ -4703,7 +4766,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:69">
+    <row r="47" spans="1:75">
       <c r="A47" s="1">
         <v>49</v>
       </c>
@@ -4713,20 +4776,23 @@
       <c r="C47" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="G47" t="s">
+        <v>88</v>
+      </c>
       <c r="Z47" t="s">
         <v>88</v>
       </c>
       <c r="AA47" t="s">
         <v>88</v>
       </c>
-      <c r="AD47" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF47" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="48" spans="1:69">
+      <c r="AE47" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:75">
       <c r="A48" s="1">
         <v>44</v>
       </c>
@@ -4757,32 +4823,32 @@
       <c r="AA48" t="s">
         <v>88</v>
       </c>
-      <c r="AD48" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF48" t="s">
-        <v>88</v>
-      </c>
-      <c r="AX48" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC48" t="s">
+      <c r="AE48" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG48" t="s">
         <v>88</v>
       </c>
       <c r="BD48" t="s">
         <v>88</v>
       </c>
-      <c r="BE48" t="s">
-        <v>88</v>
-      </c>
-      <c r="BN48" t="s">
-        <v>88</v>
-      </c>
-      <c r="BQ48" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="49" spans="1:69">
+      <c r="BI48" t="s">
+        <v>88</v>
+      </c>
+      <c r="BJ48" t="s">
+        <v>88</v>
+      </c>
+      <c r="BK48" t="s">
+        <v>88</v>
+      </c>
+      <c r="BT48" t="s">
+        <v>88</v>
+      </c>
+      <c r="BW48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:75">
       <c r="A49" s="1">
         <v>42</v>
       </c>
@@ -4792,14 +4858,14 @@
       <c r="C49" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AD49" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF49" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50" spans="1:69">
+      <c r="AE49" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG49" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:75">
       <c r="A50" s="1">
         <v>28</v>
       </c>
@@ -4818,17 +4884,17 @@
       <c r="AA50" t="s">
         <v>88</v>
       </c>
-      <c r="AD50" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF50" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC50" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="51" spans="1:69">
+      <c r="AE50" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG50" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI50" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:75">
       <c r="A51" s="1">
         <v>29</v>
       </c>
@@ -4841,14 +4907,14 @@
       <c r="U51" t="s">
         <v>88</v>
       </c>
-      <c r="AD51" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF51" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="52" spans="1:69">
+      <c r="AE51" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG51" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:75">
       <c r="A52" s="1">
         <v>48</v>
       </c>
@@ -4867,17 +4933,17 @@
       <c r="AA52" t="s">
         <v>88</v>
       </c>
-      <c r="AD52" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF52" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC52" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="53" spans="1:69">
+      <c r="AE52" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG52" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI52" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:75">
       <c r="A53" s="1">
         <v>2</v>
       </c>
@@ -4920,19 +4986,10 @@
       <c r="AA53" t="s">
         <v>88</v>
       </c>
-      <c r="AD53" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF53" t="s">
-        <v>88</v>
-      </c>
-      <c r="AX53" t="s">
-        <v>88</v>
-      </c>
-      <c r="AY53" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC53" t="s">
+      <c r="AE53" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG53" t="s">
         <v>88</v>
       </c>
       <c r="BD53" t="s">
@@ -4941,14 +4998,23 @@
       <c r="BE53" t="s">
         <v>88</v>
       </c>
-      <c r="BN53" t="s">
-        <v>88</v>
-      </c>
-      <c r="BQ53" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="54" spans="1:69">
+      <c r="BI53" t="s">
+        <v>88</v>
+      </c>
+      <c r="BJ53" t="s">
+        <v>88</v>
+      </c>
+      <c r="BK53" t="s">
+        <v>88</v>
+      </c>
+      <c r="BT53" t="s">
+        <v>88</v>
+      </c>
+      <c r="BW53" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:75">
       <c r="A54" s="1">
         <v>31</v>
       </c>
@@ -4967,20 +5033,20 @@
       <c r="AA54" t="s">
         <v>88</v>
       </c>
-      <c r="AD54" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF54" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC54" t="s">
-        <v>88</v>
-      </c>
-      <c r="BE54" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="55" spans="1:69">
+      <c r="AE54" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG54" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI54" t="s">
+        <v>88</v>
+      </c>
+      <c r="BK54" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="1:75">
       <c r="A55" s="1">
         <v>77</v>
       </c>
@@ -4996,14 +5062,14 @@
       <c r="AA55" t="s">
         <v>88</v>
       </c>
-      <c r="AF55" t="s">
-        <v>88</v>
-      </c>
-      <c r="BE55" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="56" spans="1:69">
+      <c r="AG55" t="s">
+        <v>88</v>
+      </c>
+      <c r="BK55" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:75">
       <c r="A56" s="1">
         <v>51</v>
       </c>
@@ -5031,26 +5097,26 @@
       <c r="AA56" t="s">
         <v>88</v>
       </c>
-      <c r="AD56" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF56" t="s">
-        <v>88</v>
-      </c>
-      <c r="AJ56" t="s">
+      <c r="AE56" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG56" t="s">
         <v>88</v>
       </c>
       <c r="AK56" t="s">
         <v>88</v>
       </c>
-      <c r="BA56" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC56" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="57" spans="1:69">
+      <c r="AL56" t="s">
+        <v>88</v>
+      </c>
+      <c r="BG56" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI56" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:75">
       <c r="A57" s="1">
         <v>67</v>
       </c>
@@ -5063,14 +5129,14 @@
       <c r="AA57" t="s">
         <v>88</v>
       </c>
-      <c r="AF57" t="s">
-        <v>88</v>
-      </c>
-      <c r="BE57" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="58" spans="1:69">
+      <c r="AG57" t="s">
+        <v>88</v>
+      </c>
+      <c r="BK57" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="1:75">
       <c r="A58" s="1">
         <v>24</v>
       </c>
@@ -5081,7 +5147,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:69">
+    <row r="59" spans="1:75">
       <c r="A59" s="1">
         <v>35</v>
       </c>
@@ -5103,20 +5169,20 @@
       <c r="AA59" t="s">
         <v>88</v>
       </c>
-      <c r="AD59" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF59" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC59" t="s">
-        <v>88</v>
-      </c>
-      <c r="BE59" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="60" spans="1:69">
+      <c r="AE59" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG59" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI59" t="s">
+        <v>88</v>
+      </c>
+      <c r="BK59" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:75">
       <c r="A60" s="1">
         <v>14</v>
       </c>
@@ -5135,17 +5201,17 @@
       <c r="AA60" t="s">
         <v>88</v>
       </c>
-      <c r="AD60" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF60" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC60" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="61" spans="1:69">
+      <c r="AE60" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG60" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI60" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" spans="1:75">
       <c r="A61" s="1">
         <v>25</v>
       </c>
@@ -5156,7 +5222,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:69">
+    <row r="62" spans="1:75">
       <c r="A62" s="1">
         <v>20</v>
       </c>
@@ -5175,17 +5241,17 @@
       <c r="AA62" t="s">
         <v>88</v>
       </c>
-      <c r="AD62" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF62" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC62" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="63" spans="1:69">
+      <c r="AE62" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG62" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI62" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="1:75">
       <c r="A63" s="1">
         <v>3</v>
       </c>
@@ -5204,20 +5270,20 @@
       <c r="AA63" t="s">
         <v>88</v>
       </c>
-      <c r="AD63" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF63" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC63" t="s">
-        <v>88</v>
-      </c>
-      <c r="BE63" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="64" spans="1:69">
+      <c r="AE63" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG63" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI63" t="s">
+        <v>88</v>
+      </c>
+      <c r="BK63" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64" spans="1:75">
       <c r="A64" s="1">
         <v>7</v>
       </c>
@@ -5245,32 +5311,32 @@
       <c r="AA64" t="s">
         <v>88</v>
       </c>
-      <c r="AD64" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF64" t="s">
-        <v>88</v>
-      </c>
-      <c r="AX64" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC64" t="s">
+      <c r="AE64" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG64" t="s">
         <v>88</v>
       </c>
       <c r="BD64" t="s">
         <v>88</v>
       </c>
-      <c r="BE64" t="s">
-        <v>88</v>
-      </c>
-      <c r="BN64" t="s">
-        <v>88</v>
-      </c>
-      <c r="BQ64" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="65" spans="1:57">
+      <c r="BI64" t="s">
+        <v>88</v>
+      </c>
+      <c r="BJ64" t="s">
+        <v>88</v>
+      </c>
+      <c r="BK64" t="s">
+        <v>88</v>
+      </c>
+      <c r="BT64" t="s">
+        <v>88</v>
+      </c>
+      <c r="BW64" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="1:63">
       <c r="A65" s="1">
         <v>26</v>
       </c>
@@ -5292,20 +5358,20 @@
       <c r="AA65" t="s">
         <v>88</v>
       </c>
-      <c r="AD65" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF65" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC65" t="s">
-        <v>88</v>
-      </c>
-      <c r="BE65" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="66" spans="1:57">
+      <c r="AE65" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG65" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI65" t="s">
+        <v>88</v>
+      </c>
+      <c r="BK65" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:63">
       <c r="A66" s="1">
         <v>43</v>
       </c>
@@ -5316,7 +5382,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="67" spans="1:57">
+    <row r="67" spans="1:63">
       <c r="A67" s="1">
         <v>23</v>
       </c>
@@ -5335,17 +5401,17 @@
       <c r="AA67" t="s">
         <v>88</v>
       </c>
-      <c r="AD67" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF67" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC67" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="68" spans="1:57">
+      <c r="AE67" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG67" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI67" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="1:63">
       <c r="A68" s="1">
         <v>50</v>
       </c>
@@ -5364,17 +5430,17 @@
       <c r="AA68" t="s">
         <v>88</v>
       </c>
-      <c r="AD68" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF68" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC68" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="69" spans="1:57">
+      <c r="AE68" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG68" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI68" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:63">
       <c r="A69" s="1">
         <v>32</v>
       </c>
@@ -5393,17 +5459,17 @@
       <c r="AA69" t="s">
         <v>88</v>
       </c>
-      <c r="AD69" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF69" t="s">
-        <v>88</v>
-      </c>
-      <c r="BC69" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="70" spans="1:57">
+      <c r="AE69" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG69" t="s">
+        <v>88</v>
+      </c>
+      <c r="BI69" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="70" spans="1:63">
       <c r="A70" s="1">
         <v>71</v>
       </c>
@@ -5414,7 +5480,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="1:57">
+    <row r="71" spans="1:63">
       <c r="A71" s="1">
         <v>76</v>
       </c>
@@ -5425,7 +5491,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="72" spans="1:57">
+    <row r="72" spans="1:63">
       <c r="A72" s="1">
         <v>73</v>
       </c>
@@ -5436,7 +5502,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="73" spans="1:57">
+    <row r="73" spans="1:63">
       <c r="A73" s="1">
         <v>57</v>
       </c>
@@ -5447,7 +5513,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:57">
+    <row r="74" spans="1:63">
       <c r="A74" s="1">
         <v>74</v>
       </c>
@@ -5458,7 +5524,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="75" spans="1:57">
+    <row r="75" spans="1:63">
       <c r="A75" s="1">
         <v>53</v>
       </c>
@@ -5469,7 +5535,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:57">
+    <row r="76" spans="1:63">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -5480,7 +5546,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="1:57">
+    <row r="77" spans="1:63">
       <c r="A77" s="1">
         <v>72</v>
       </c>
@@ -5935,6 +6001,9 @@
       <c r="E15" s="3">
         <v>45229</v>
       </c>
+      <c r="F15" s="3">
+        <v>45232</v>
+      </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1">
@@ -6697,6 +6766,9 @@
       </c>
       <c r="G47" s="3">
         <v>45216</v>
+      </c>
+      <c r="I47" s="3">
+        <v>45237</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -7411,13 +7483,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BV77"/>
+  <dimension ref="A1:CB77"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:74">
+    <row r="1" spans="1:80">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7503,16 +7575,16 @@
         <v>111</v>
       </c>
       <c r="AD1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="AF1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>114</v>
@@ -7578,25 +7650,25 @@
         <v>134</v>
       </c>
       <c r="BC1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="BH1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="BI1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="BH1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="BI1" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="BJ1" s="1" t="s">
         <v>141</v>
@@ -7637,8 +7709,26 @@
       <c r="BV1" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="2" spans="1:74">
+      <c r="BW1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:80">
       <c r="A2" s="1">
         <v>79</v>
       </c>
@@ -7649,7 +7739,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:74">
+    <row r="3" spans="1:80">
       <c r="A3" s="1">
         <v>58</v>
       </c>
@@ -7668,17 +7758,17 @@
       <c r="AA3" s="3">
         <v>45166</v>
       </c>
-      <c r="AD3" s="3">
+      <c r="AE3" s="3">
         <v>45165</v>
       </c>
-      <c r="AF3" s="3">
+      <c r="AG3" s="3">
         <v>45166</v>
       </c>
-      <c r="BC3" s="3">
+      <c r="BI3" s="3">
         <v>45168</v>
       </c>
     </row>
-    <row r="4" spans="1:74">
+    <row r="4" spans="1:80">
       <c r="A4" s="1">
         <v>46</v>
       </c>
@@ -7688,14 +7778,14 @@
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="3">
+      <c r="AE4" s="3">
         <v>45168</v>
       </c>
-      <c r="AF4" s="3">
+      <c r="AG4" s="3">
         <v>45177</v>
       </c>
     </row>
-    <row r="5" spans="1:74">
+    <row r="5" spans="1:80">
       <c r="A5" s="1">
         <v>21</v>
       </c>
@@ -7706,7 +7796,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:74">
+    <row r="6" spans="1:80">
       <c r="A6" s="1">
         <v>12</v>
       </c>
@@ -7717,7 +7807,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:74">
+    <row r="7" spans="1:80">
       <c r="A7" s="1">
         <v>27</v>
       </c>
@@ -7739,20 +7829,20 @@
       <c r="AA7" s="3">
         <v>45167</v>
       </c>
-      <c r="AD7" s="3">
+      <c r="AE7" s="3">
         <v>45167</v>
       </c>
-      <c r="AF7" s="3">
+      <c r="AG7" s="3">
         <v>45166</v>
       </c>
-      <c r="BC7" s="3">
+      <c r="BI7" s="3">
         <v>45168</v>
       </c>
-      <c r="BE7" s="3">
+      <c r="BK7" s="3">
         <v>45165</v>
       </c>
     </row>
-    <row r="8" spans="1:74">
+    <row r="8" spans="1:80">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -7829,127 +7919,145 @@
         <v>45046</v>
       </c>
       <c r="AD8" s="3">
+        <v>45235</v>
+      </c>
+      <c r="AE8" s="3">
         <v>44911</v>
       </c>
-      <c r="AE8" s="3">
+      <c r="AF8" s="3">
         <v>44938</v>
       </c>
-      <c r="AF8" s="3">
+      <c r="AG8" s="3">
         <v>44836</v>
       </c>
-      <c r="AG8" s="3">
+      <c r="AH8" s="3">
         <v>45024</v>
       </c>
-      <c r="AH8" s="3">
+      <c r="AI8" s="3">
         <v>45002</v>
       </c>
-      <c r="AI8" s="3">
+      <c r="AJ8" s="3">
         <v>45074</v>
       </c>
-      <c r="AL8" s="3">
+      <c r="AM8" s="3">
         <v>45102</v>
       </c>
-      <c r="AM8" s="3">
+      <c r="AN8" s="3">
+        <v>45232</v>
+      </c>
+      <c r="AO8" s="3">
+        <v>45232</v>
+      </c>
+      <c r="AP8" s="3">
         <v>45005</v>
       </c>
-      <c r="AN8" s="3">
+      <c r="AQ8" s="3">
         <v>45136</v>
       </c>
-      <c r="AO8" s="3">
+      <c r="AR8" s="3">
         <v>45158</v>
       </c>
-      <c r="AP8" s="3">
+      <c r="AS8" s="3">
+        <v>45229</v>
+      </c>
+      <c r="AT8" s="3">
         <v>45074</v>
       </c>
-      <c r="AQ8" s="3">
+      <c r="AU8" s="3">
         <v>45041</v>
       </c>
-      <c r="AR8" s="3">
+      <c r="AV8" s="3">
         <v>45199</v>
-      </c>
-      <c r="AS8" s="3">
-        <v>45167</v>
-      </c>
-      <c r="AT8" s="3">
-        <v>45076</v>
-      </c>
-      <c r="AU8" s="3">
-        <v>45138</v>
-      </c>
-      <c r="AV8" s="3">
-        <v>45046</v>
       </c>
       <c r="AW8" s="3">
         <v>45167</v>
       </c>
+      <c r="AX8" s="3">
+        <v>45076</v>
+      </c>
       <c r="AY8" s="3">
+        <v>45138</v>
+      </c>
+      <c r="AZ8" s="3">
+        <v>45046</v>
+      </c>
+      <c r="BA8" s="3">
+        <v>45230</v>
+      </c>
+      <c r="BB8" s="3">
+        <v>45230</v>
+      </c>
+      <c r="BC8" s="3">
+        <v>45167</v>
+      </c>
+      <c r="BE8" s="3">
         <v>45015</v>
       </c>
-      <c r="AZ8" s="3">
+      <c r="BF8" s="3">
         <v>45002</v>
       </c>
-      <c r="BB8" s="3">
+      <c r="BH8" s="3">
         <v>45041</v>
       </c>
-      <c r="BC8" s="3">
+      <c r="BI8" s="3">
         <v>45157</v>
       </c>
-      <c r="BD8" s="3">
+      <c r="BJ8" s="3">
         <v>45074</v>
       </c>
-      <c r="BF8" s="3">
+      <c r="BL8" s="3">
         <v>45046</v>
       </c>
-      <c r="BG8" s="3">
+      <c r="BM8" s="3">
         <v>45166</v>
       </c>
-      <c r="BH8" s="3">
+      <c r="BN8" s="3">
         <v>45146</v>
       </c>
-      <c r="BI8" s="3">
+      <c r="BO8" s="3">
         <v>45075</v>
       </c>
-      <c r="BJ8" s="3">
+      <c r="BP8" s="3">
         <v>45224</v>
       </c>
-      <c r="BK8" s="3">
+      <c r="BQ8" s="3">
         <v>45224</v>
       </c>
-      <c r="BL8" s="3">
+      <c r="BR8" s="3">
         <v>45224</v>
       </c>
-      <c r="BM8" s="3">
+      <c r="BS8" s="3">
         <v>45224</v>
       </c>
-      <c r="BN8" s="3">
+      <c r="BT8" s="3">
         <v>44864</v>
       </c>
-      <c r="BO8" s="3">
+      <c r="BU8" s="3">
         <v>45199</v>
       </c>
-      <c r="BP8" s="3">
+      <c r="BV8" s="3">
         <v>45076</v>
       </c>
-      <c r="BQ8" s="3">
+      <c r="BW8" s="3">
         <v>44933</v>
       </c>
-      <c r="BR8" s="3">
+      <c r="BX8" s="3">
         <v>45047</v>
       </c>
-      <c r="BS8" s="3">
+      <c r="BY8" s="3">
         <v>45047</v>
       </c>
-      <c r="BT8" s="3">
+      <c r="BZ8" s="3">
         <v>45074</v>
       </c>
-      <c r="BU8" s="3">
+      <c r="CA8" s="3">
         <v>45135</v>
       </c>
-      <c r="BV8" s="3">
+      <c r="CB8" s="3">
         <v>45046</v>
       </c>
     </row>
-    <row r="9" spans="1:74">
+    <row r="9" spans="1:80">
       <c r="A9" s="1">
         <v>18</v>
       </c>
@@ -7983,29 +8091,29 @@
       <c r="AA9" s="3">
         <v>45148</v>
       </c>
-      <c r="AD9" s="3">
+      <c r="AE9" s="3">
         <v>45075</v>
       </c>
-      <c r="AF9" s="3">
+      <c r="AG9" s="3">
         <v>45148</v>
       </c>
-      <c r="AI9" s="3">
+      <c r="AJ9" s="3">
         <v>45023</v>
       </c>
-      <c r="AY9" s="3">
+      <c r="BE9" s="3">
         <v>45015</v>
       </c>
-      <c r="BC9" s="3">
+      <c r="BI9" s="3">
         <v>45152</v>
       </c>
-      <c r="BD9" s="3">
+      <c r="BJ9" s="3">
         <v>44855</v>
       </c>
-      <c r="BQ9" s="3">
+      <c r="BW9" s="3">
         <v>45023</v>
       </c>
     </row>
-    <row r="10" spans="1:74">
+    <row r="10" spans="1:80">
       <c r="A10" s="1">
         <v>19</v>
       </c>
@@ -8024,20 +8132,20 @@
       <c r="AA10" s="3">
         <v>45153</v>
       </c>
-      <c r="AD10" s="3">
+      <c r="AE10" s="3">
         <v>45155</v>
       </c>
-      <c r="AF10" s="3">
+      <c r="AG10" s="3">
         <v>45152</v>
       </c>
-      <c r="BC10" s="3">
+      <c r="BI10" s="3">
         <v>45155</v>
       </c>
-      <c r="BE10" s="3">
+      <c r="BK10" s="3">
         <v>45148</v>
       </c>
     </row>
-    <row r="11" spans="1:74">
+    <row r="11" spans="1:80">
       <c r="A11" s="1">
         <v>16</v>
       </c>
@@ -8059,17 +8167,17 @@
       <c r="AA11" s="3">
         <v>45167</v>
       </c>
-      <c r="AD11" s="3">
+      <c r="AE11" s="3">
         <v>45167</v>
       </c>
-      <c r="AF11" s="3">
+      <c r="AG11" s="3">
         <v>45166</v>
       </c>
-      <c r="BC11" s="3">
+      <c r="BI11" s="3">
         <v>45168</v>
       </c>
     </row>
-    <row r="12" spans="1:74">
+    <row r="12" spans="1:80">
       <c r="A12" s="1">
         <v>40</v>
       </c>
@@ -8100,32 +8208,32 @@
       <c r="AA12" s="3">
         <v>45149</v>
       </c>
-      <c r="AD12" s="3">
+      <c r="AE12" s="3">
         <v>45153</v>
       </c>
-      <c r="AF12" s="3">
+      <c r="AG12" s="3">
         <v>45148</v>
       </c>
-      <c r="AX12" s="3">
+      <c r="BD12" s="3">
         <v>45153</v>
       </c>
-      <c r="BC12" s="3">
+      <c r="BI12" s="3">
         <v>45155</v>
       </c>
-      <c r="BD12" s="3">
+      <c r="BJ12" s="3">
         <v>45154</v>
       </c>
-      <c r="BE12" s="3">
+      <c r="BK12" s="3">
         <v>45148</v>
       </c>
-      <c r="BN12" s="3">
+      <c r="BT12" s="3">
         <v>45153</v>
       </c>
-      <c r="BQ12" s="3">
+      <c r="BW12" s="3">
         <v>45154</v>
       </c>
     </row>
-    <row r="13" spans="1:74">
+    <row r="13" spans="1:80">
       <c r="A13" s="1">
         <v>6</v>
       </c>
@@ -8144,17 +8252,17 @@
       <c r="AA13" s="3">
         <v>45169</v>
       </c>
-      <c r="AD13" s="3">
+      <c r="AE13" s="3">
         <v>45162</v>
       </c>
-      <c r="AF13" s="3">
+      <c r="AG13" s="3">
         <v>45169</v>
       </c>
-      <c r="BC13" s="3">
+      <c r="BI13" s="3">
         <v>45172</v>
       </c>
     </row>
-    <row r="14" spans="1:74">
+    <row r="14" spans="1:80">
       <c r="A14" s="1">
         <v>59</v>
       </c>
@@ -8173,17 +8281,17 @@
       <c r="AA14" s="3">
         <v>45167</v>
       </c>
-      <c r="AD14" s="3">
+      <c r="AE14" s="3">
         <v>45167</v>
       </c>
-      <c r="AF14" s="3">
+      <c r="AG14" s="3">
         <v>45167</v>
       </c>
-      <c r="BC14" s="3">
+      <c r="BI14" s="3">
         <v>45168</v>
       </c>
     </row>
-    <row r="15" spans="1:74">
+    <row r="15" spans="1:80">
       <c r="A15" s="1">
         <v>70</v>
       </c>
@@ -8193,14 +8301,17 @@
       <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AD15" s="3">
+      <c r="AA15" s="3">
+        <v>45232</v>
+      </c>
+      <c r="AE15" s="3">
         <v>45195</v>
       </c>
-      <c r="AF15" s="3">
+      <c r="AG15" s="3">
         <v>45229</v>
       </c>
     </row>
-    <row r="16" spans="1:74">
+    <row r="16" spans="1:80">
       <c r="A16" s="1">
         <v>47</v>
       </c>
@@ -8219,17 +8330,17 @@
       <c r="AA16" s="3">
         <v>45165</v>
       </c>
-      <c r="AD16" s="3">
+      <c r="AE16" s="3">
         <v>45167</v>
       </c>
-      <c r="AF16" s="3">
+      <c r="AG16" s="3">
         <v>45165</v>
       </c>
-      <c r="BC16" s="3">
+      <c r="BI16" s="3">
         <v>45167</v>
       </c>
     </row>
-    <row r="17" spans="1:66">
+    <row r="17" spans="1:72">
       <c r="A17" s="1">
         <v>54</v>
       </c>
@@ -8240,7 +8351,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:66">
+    <row r="18" spans="1:72">
       <c r="A18" s="1">
         <v>0</v>
       </c>
@@ -8259,17 +8370,17 @@
       <c r="AA18" s="3">
         <v>45145</v>
       </c>
-      <c r="AD18" s="3">
+      <c r="AE18" s="3">
         <v>45159</v>
       </c>
-      <c r="AF18" s="3">
+      <c r="AG18" s="3">
         <v>45138</v>
       </c>
-      <c r="BC18" s="3">
+      <c r="BI18" s="3">
         <v>45165</v>
       </c>
     </row>
-    <row r="19" spans="1:66">
+    <row r="19" spans="1:72">
       <c r="A19" s="1">
         <v>41</v>
       </c>
@@ -8288,17 +8399,17 @@
       <c r="AA19" s="3">
         <v>45160</v>
       </c>
-      <c r="AD19" s="3">
+      <c r="AE19" s="3">
         <v>45160</v>
       </c>
-      <c r="AF19" s="3">
+      <c r="AG19" s="3">
         <v>45161</v>
       </c>
-      <c r="BC19" s="3">
+      <c r="BI19" s="3">
         <v>45164</v>
       </c>
     </row>
-    <row r="20" spans="1:66">
+    <row r="20" spans="1:72">
       <c r="A20" s="1">
         <v>9</v>
       </c>
@@ -8320,20 +8431,20 @@
       <c r="AA20" s="3">
         <v>45160</v>
       </c>
-      <c r="AD20" s="3">
+      <c r="AE20" s="3">
         <v>45164</v>
       </c>
-      <c r="AF20" s="3">
+      <c r="AG20" s="3">
         <v>45158</v>
       </c>
-      <c r="BC20" s="3">
+      <c r="BI20" s="3">
         <v>45165</v>
       </c>
-      <c r="BE20" s="3">
+      <c r="BK20" s="3">
         <v>45152</v>
       </c>
     </row>
-    <row r="21" spans="1:66">
+    <row r="21" spans="1:72">
       <c r="A21" s="1">
         <v>30</v>
       </c>
@@ -8344,7 +8455,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:66">
+    <row r="22" spans="1:72">
       <c r="A22" s="1">
         <v>4</v>
       </c>
@@ -8363,17 +8474,17 @@
       <c r="AA22" s="3">
         <v>45163</v>
       </c>
-      <c r="AD22" s="3">
+      <c r="AE22" s="3">
         <v>45162</v>
       </c>
-      <c r="AF22" s="3">
+      <c r="AG22" s="3">
         <v>45163</v>
       </c>
-      <c r="BC22" s="3">
+      <c r="BI22" s="3">
         <v>45165</v>
       </c>
     </row>
-    <row r="23" spans="1:66">
+    <row r="23" spans="1:72">
       <c r="A23" s="1">
         <v>64</v>
       </c>
@@ -8384,7 +8495,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:66">
+    <row r="24" spans="1:72">
       <c r="A24" s="1">
         <v>10</v>
       </c>
@@ -8403,20 +8514,20 @@
       <c r="AA24" s="3">
         <v>45154</v>
       </c>
-      <c r="AD24" s="3">
+      <c r="AE24" s="3">
         <v>45159</v>
       </c>
-      <c r="AF24" s="3">
+      <c r="AG24" s="3">
         <v>45154</v>
       </c>
-      <c r="BC24" s="3">
+      <c r="BI24" s="3">
         <v>45160</v>
       </c>
-      <c r="BE24" s="3">
+      <c r="BK24" s="3">
         <v>45153</v>
       </c>
     </row>
-    <row r="25" spans="1:66">
+    <row r="25" spans="1:72">
       <c r="A25" s="1">
         <v>33</v>
       </c>
@@ -8435,20 +8546,20 @@
       <c r="AA25" s="3">
         <v>45161</v>
       </c>
-      <c r="AD25" s="3">
+      <c r="AE25" s="3">
         <v>45159</v>
       </c>
-      <c r="AF25" s="3">
+      <c r="AG25" s="3">
         <v>45160</v>
       </c>
-      <c r="BC25" s="3">
+      <c r="BI25" s="3">
         <v>45166</v>
       </c>
-      <c r="BE25" s="3">
+      <c r="BK25" s="3">
         <v>45145</v>
       </c>
     </row>
-    <row r="26" spans="1:66">
+    <row r="26" spans="1:72">
       <c r="A26" s="1">
         <v>52</v>
       </c>
@@ -8459,7 +8570,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:66">
+    <row r="27" spans="1:72">
       <c r="A27" s="1">
         <v>62</v>
       </c>
@@ -8478,17 +8589,17 @@
       <c r="AA27" s="3">
         <v>45224</v>
       </c>
-      <c r="AD27" s="3">
+      <c r="AE27" s="3">
         <v>45222</v>
       </c>
-      <c r="AF27" s="3">
+      <c r="AG27" s="3">
         <v>45223</v>
       </c>
-      <c r="BC27" s="3">
+      <c r="BI27" s="3">
         <v>45226</v>
       </c>
     </row>
-    <row r="28" spans="1:66">
+    <row r="28" spans="1:72">
       <c r="A28" s="1">
         <v>69</v>
       </c>
@@ -8499,7 +8610,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:66">
+    <row r="29" spans="1:72">
       <c r="A29" s="1">
         <v>38</v>
       </c>
@@ -8518,17 +8629,17 @@
       <c r="AA29" s="3">
         <v>45165</v>
       </c>
-      <c r="AD29" s="3">
+      <c r="AE29" s="3">
         <v>45164</v>
       </c>
-      <c r="AF29" s="3">
+      <c r="AG29" s="3">
         <v>45164</v>
       </c>
-      <c r="BC29" s="3">
+      <c r="BI29" s="3">
         <v>45168</v>
       </c>
     </row>
-    <row r="30" spans="1:66">
+    <row r="30" spans="1:72">
       <c r="A30" s="1">
         <v>15</v>
       </c>
@@ -8547,17 +8658,17 @@
       <c r="AA30" s="3">
         <v>45168</v>
       </c>
-      <c r="AD30" s="3">
+      <c r="AE30" s="3">
         <v>45166</v>
       </c>
-      <c r="AF30" s="3">
+      <c r="AG30" s="3">
         <v>45167</v>
       </c>
-      <c r="BC30" s="3">
+      <c r="BI30" s="3">
         <v>45169</v>
       </c>
     </row>
-    <row r="31" spans="1:66">
+    <row r="31" spans="1:72">
       <c r="A31" s="1">
         <v>37</v>
       </c>
@@ -8576,23 +8687,23 @@
       <c r="AA31" s="3">
         <v>45166</v>
       </c>
-      <c r="AD31" s="3">
+      <c r="AE31" s="3">
         <v>45166</v>
       </c>
-      <c r="AF31" s="3">
+      <c r="AG31" s="3">
         <v>45166</v>
       </c>
-      <c r="AX31" s="3">
+      <c r="BD31" s="3">
         <v>45182</v>
       </c>
-      <c r="BC31" s="3">
+      <c r="BI31" s="3">
         <v>45166</v>
       </c>
-      <c r="BN31" s="3">
+      <c r="BT31" s="3">
         <v>45182</v>
       </c>
     </row>
-    <row r="32" spans="1:66">
+    <row r="32" spans="1:72">
       <c r="A32" s="1">
         <v>11</v>
       </c>
@@ -8611,17 +8722,17 @@
       <c r="AA32" s="3">
         <v>45155</v>
       </c>
-      <c r="AD32" s="3">
+      <c r="AE32" s="3">
         <v>45167</v>
       </c>
-      <c r="AF32" s="3">
+      <c r="AG32" s="3">
         <v>45154</v>
       </c>
-      <c r="BC32" s="3">
+      <c r="BI32" s="3">
         <v>45167</v>
       </c>
     </row>
-    <row r="33" spans="1:69">
+    <row r="33" spans="1:75">
       <c r="A33" s="1">
         <v>56</v>
       </c>
@@ -8640,17 +8751,17 @@
       <c r="AA33" s="3">
         <v>45219</v>
       </c>
-      <c r="AD33" s="3">
+      <c r="AE33" s="3">
         <v>45219</v>
       </c>
-      <c r="AF33" s="3">
+      <c r="AG33" s="3">
         <v>45219</v>
       </c>
-      <c r="BC33" s="3">
+      <c r="BI33" s="3">
         <v>45220</v>
       </c>
     </row>
-    <row r="34" spans="1:69">
+    <row r="34" spans="1:75">
       <c r="A34" s="1">
         <v>17</v>
       </c>
@@ -8669,17 +8780,17 @@
       <c r="AA34" s="3">
         <v>45167</v>
       </c>
-      <c r="AD34" s="3">
+      <c r="AE34" s="3">
         <v>45168</v>
       </c>
-      <c r="AF34" s="3">
+      <c r="AG34" s="3">
         <v>45167</v>
       </c>
-      <c r="BC34" s="3">
+      <c r="BI34" s="3">
         <v>45169</v>
       </c>
     </row>
-    <row r="35" spans="1:69">
+    <row r="35" spans="1:75">
       <c r="A35" s="1">
         <v>22</v>
       </c>
@@ -8695,20 +8806,20 @@
       <c r="AA35" s="3">
         <v>45181</v>
       </c>
-      <c r="AD35" s="3">
+      <c r="AE35" s="3">
         <v>45168</v>
       </c>
-      <c r="AF35" s="3">
+      <c r="AG35" s="3">
         <v>45177</v>
       </c>
-      <c r="BC35" s="3">
+      <c r="BI35" s="3">
         <v>45199</v>
       </c>
-      <c r="BE35" s="3">
+      <c r="BK35" s="3">
         <v>45158</v>
       </c>
     </row>
-    <row r="36" spans="1:69">
+    <row r="36" spans="1:75">
       <c r="A36" s="1">
         <v>78</v>
       </c>
@@ -8719,7 +8830,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:69">
+    <row r="37" spans="1:75">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -8738,17 +8849,17 @@
       <c r="AA37" s="3">
         <v>45161</v>
       </c>
-      <c r="AD37" s="3">
+      <c r="AE37" s="3">
         <v>45159</v>
       </c>
-      <c r="AF37" s="3">
+      <c r="AG37" s="3">
         <v>45160</v>
       </c>
-      <c r="BC37" s="3">
+      <c r="BI37" s="3">
         <v>45163</v>
       </c>
     </row>
-    <row r="38" spans="1:69">
+    <row r="38" spans="1:75">
       <c r="A38" s="1">
         <v>34</v>
       </c>
@@ -8767,17 +8878,17 @@
       <c r="AA38" s="3">
         <v>45160</v>
       </c>
-      <c r="AD38" s="3">
+      <c r="AE38" s="3">
         <v>45162</v>
       </c>
-      <c r="AF38" s="3">
+      <c r="AG38" s="3">
         <v>45159</v>
       </c>
-      <c r="BC38" s="3">
+      <c r="BI38" s="3">
         <v>45166</v>
       </c>
     </row>
-    <row r="39" spans="1:69">
+    <row r="39" spans="1:75">
       <c r="A39" s="1">
         <v>13</v>
       </c>
@@ -8796,17 +8907,17 @@
       <c r="AA39" s="3">
         <v>45191</v>
       </c>
-      <c r="AD39" s="3">
+      <c r="AE39" s="3">
         <v>45182</v>
       </c>
-      <c r="AF39" s="3">
+      <c r="AG39" s="3">
         <v>45183</v>
       </c>
-      <c r="BC39" s="3">
+      <c r="BI39" s="3">
         <v>45192</v>
       </c>
     </row>
-    <row r="40" spans="1:69">
+    <row r="40" spans="1:75">
       <c r="A40" s="1">
         <v>65</v>
       </c>
@@ -8825,17 +8936,17 @@
       <c r="AA40" s="3">
         <v>45207</v>
       </c>
-      <c r="AD40" s="3">
+      <c r="AE40" s="3">
         <v>45198</v>
       </c>
-      <c r="AF40" s="3">
+      <c r="AG40" s="3">
         <v>45199</v>
       </c>
-      <c r="BC40" s="3">
+      <c r="BI40" s="3">
         <v>45208</v>
       </c>
     </row>
-    <row r="41" spans="1:69">
+    <row r="41" spans="1:75">
       <c r="A41" s="1">
         <v>66</v>
       </c>
@@ -8848,14 +8959,14 @@
       <c r="Z41" s="3">
         <v>45168</v>
       </c>
-      <c r="AF41" s="3">
+      <c r="AG41" s="3">
         <v>45166</v>
       </c>
-      <c r="BE41" s="3">
+      <c r="BK41" s="3">
         <v>45167</v>
       </c>
     </row>
-    <row r="42" spans="1:69">
+    <row r="42" spans="1:75">
       <c r="A42" s="1">
         <v>68</v>
       </c>
@@ -8874,17 +8985,17 @@
       <c r="AA42" s="3">
         <v>45208</v>
       </c>
-      <c r="AD42" s="3">
+      <c r="AE42" s="3">
         <v>45195</v>
       </c>
-      <c r="AF42" s="3">
+      <c r="AG42" s="3">
         <v>45208</v>
       </c>
-      <c r="BC42" s="3">
+      <c r="BI42" s="3">
         <v>45220</v>
       </c>
     </row>
-    <row r="43" spans="1:69">
+    <row r="43" spans="1:75">
       <c r="A43" s="1">
         <v>8</v>
       </c>
@@ -8903,17 +9014,17 @@
       <c r="AA43" s="3">
         <v>45155</v>
       </c>
-      <c r="AD43" s="3">
+      <c r="AE43" s="3">
         <v>45147</v>
       </c>
-      <c r="AF43" s="3">
+      <c r="AG43" s="3">
         <v>45154</v>
       </c>
-      <c r="BC43" s="3">
+      <c r="BI43" s="3">
         <v>45158</v>
       </c>
     </row>
-    <row r="44" spans="1:69">
+    <row r="44" spans="1:75">
       <c r="A44" s="1">
         <v>60</v>
       </c>
@@ -8932,17 +9043,17 @@
       <c r="AA44" s="3">
         <v>45174</v>
       </c>
-      <c r="AD44" s="3">
+      <c r="AE44" s="3">
         <v>45169</v>
       </c>
-      <c r="AF44" s="3">
+      <c r="AG44" s="3">
         <v>45169</v>
       </c>
-      <c r="BC44" s="3">
+      <c r="BI44" s="3">
         <v>45197</v>
       </c>
     </row>
-    <row r="45" spans="1:69">
+    <row r="45" spans="1:75">
       <c r="A45" s="1">
         <v>61</v>
       </c>
@@ -8953,7 +9064,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:69">
+    <row r="46" spans="1:75">
       <c r="A46" s="1">
         <v>63</v>
       </c>
@@ -8964,7 +9075,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:69">
+    <row r="47" spans="1:75">
       <c r="A47" s="1">
         <v>49</v>
       </c>
@@ -8974,20 +9085,23 @@
       <c r="C47" s="2" t="s">
         <v>57</v>
       </c>
+      <c r="G47" s="3">
+        <v>45237</v>
+      </c>
       <c r="Z47" s="3">
         <v>45216</v>
       </c>
       <c r="AA47" s="3">
         <v>45177</v>
       </c>
-      <c r="AD47" s="3">
+      <c r="AE47" s="3">
         <v>45165</v>
       </c>
-      <c r="AF47" s="3">
+      <c r="AG47" s="3">
         <v>45173</v>
       </c>
     </row>
-    <row r="48" spans="1:69">
+    <row r="48" spans="1:75">
       <c r="A48" s="1">
         <v>44</v>
       </c>
@@ -9018,32 +9132,32 @@
       <c r="AA48" s="3">
         <v>44829</v>
       </c>
-      <c r="AD48" s="3">
+      <c r="AE48" s="3">
         <v>44908</v>
       </c>
-      <c r="AF48" s="3">
+      <c r="AG48" s="3">
         <v>44829</v>
       </c>
-      <c r="AX48" s="3">
+      <c r="BD48" s="3">
         <v>44910</v>
       </c>
-      <c r="BC48" s="3">
+      <c r="BI48" s="3">
         <v>44915</v>
       </c>
-      <c r="BD48" s="3">
+      <c r="BJ48" s="3">
         <v>44911</v>
       </c>
-      <c r="BE48" s="3">
+      <c r="BK48" s="3">
         <v>44915</v>
       </c>
-      <c r="BN48" s="3">
+      <c r="BT48" s="3">
         <v>44862</v>
       </c>
-      <c r="BQ48" s="3">
+      <c r="BW48" s="3">
         <v>44911</v>
       </c>
     </row>
-    <row r="49" spans="1:69">
+    <row r="49" spans="1:75">
       <c r="A49" s="1">
         <v>42</v>
       </c>
@@ -9053,14 +9167,14 @@
       <c r="C49" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AD49" s="3">
+      <c r="AE49" s="3">
         <v>45183</v>
       </c>
-      <c r="AF49" s="3">
+      <c r="AG49" s="3">
         <v>45166</v>
       </c>
     </row>
-    <row r="50" spans="1:69">
+    <row r="50" spans="1:75">
       <c r="A50" s="1">
         <v>28</v>
       </c>
@@ -9079,17 +9193,17 @@
       <c r="AA50" s="3">
         <v>45169</v>
       </c>
-      <c r="AD50" s="3">
+      <c r="AE50" s="3">
         <v>45169</v>
       </c>
-      <c r="AF50" s="3">
+      <c r="AG50" s="3">
         <v>45168</v>
       </c>
-      <c r="BC50" s="3">
+      <c r="BI50" s="3">
         <v>45169</v>
       </c>
     </row>
-    <row r="51" spans="1:69">
+    <row r="51" spans="1:75">
       <c r="A51" s="1">
         <v>29</v>
       </c>
@@ -9102,14 +9216,14 @@
       <c r="U51" s="3">
         <v>44852</v>
       </c>
-      <c r="AD51" s="3">
+      <c r="AE51" s="3">
         <v>45216</v>
       </c>
-      <c r="AF51" s="3">
+      <c r="AG51" s="3">
         <v>44911</v>
       </c>
     </row>
-    <row r="52" spans="1:69">
+    <row r="52" spans="1:75">
       <c r="A52" s="1">
         <v>48</v>
       </c>
@@ -9128,17 +9242,17 @@
       <c r="AA52" s="3">
         <v>45170</v>
       </c>
-      <c r="AD52" s="3">
+      <c r="AE52" s="3">
         <v>45168</v>
       </c>
-      <c r="AF52" s="3">
+      <c r="AG52" s="3">
         <v>45168</v>
       </c>
-      <c r="BC52" s="3">
+      <c r="BI52" s="3">
         <v>45170</v>
       </c>
     </row>
-    <row r="53" spans="1:69">
+    <row r="53" spans="1:75">
       <c r="A53" s="1">
         <v>2</v>
       </c>
@@ -9181,35 +9295,35 @@
       <c r="AA53" s="3">
         <v>44939</v>
       </c>
-      <c r="AD53" s="3">
+      <c r="AE53" s="3">
         <v>44941</v>
       </c>
-      <c r="AF53" s="3">
+      <c r="AG53" s="3">
         <v>44939</v>
       </c>
-      <c r="AX53" s="3">
+      <c r="BD53" s="3">
         <v>44942</v>
       </c>
-      <c r="AY53" s="3">
+      <c r="BE53" s="3">
         <v>45015</v>
       </c>
-      <c r="BC53" s="3">
+      <c r="BI53" s="3">
         <v>44951</v>
       </c>
-      <c r="BD53" s="3">
+      <c r="BJ53" s="3">
         <v>44939</v>
       </c>
-      <c r="BE53" s="3">
+      <c r="BK53" s="3">
         <v>44936</v>
       </c>
-      <c r="BN53" s="3">
+      <c r="BT53" s="3">
         <v>44941</v>
       </c>
-      <c r="BQ53" s="3">
+      <c r="BW53" s="3">
         <v>44948</v>
       </c>
     </row>
-    <row r="54" spans="1:69">
+    <row r="54" spans="1:75">
       <c r="A54" s="1">
         <v>31</v>
       </c>
@@ -9228,20 +9342,20 @@
       <c r="AA54" s="3">
         <v>45155</v>
       </c>
-      <c r="AD54" s="3">
+      <c r="AE54" s="3">
         <v>45156</v>
       </c>
-      <c r="AF54" s="3">
+      <c r="AG54" s="3">
         <v>45151</v>
       </c>
-      <c r="BC54" s="3">
+      <c r="BI54" s="3">
         <v>45157</v>
       </c>
-      <c r="BE54" s="3">
+      <c r="BK54" s="3">
         <v>45150</v>
       </c>
     </row>
-    <row r="55" spans="1:69">
+    <row r="55" spans="1:75">
       <c r="A55" s="1">
         <v>77</v>
       </c>
@@ -9257,14 +9371,14 @@
       <c r="AA55" s="3">
         <v>45214</v>
       </c>
-      <c r="AF55" s="3">
+      <c r="AG55" s="3">
         <v>45199</v>
       </c>
-      <c r="BE55" s="3">
+      <c r="BK55" s="3">
         <v>45164</v>
       </c>
     </row>
-    <row r="56" spans="1:69">
+    <row r="56" spans="1:75">
       <c r="A56" s="1">
         <v>51</v>
       </c>
@@ -9292,26 +9406,26 @@
       <c r="AA56" s="3">
         <v>45168</v>
       </c>
-      <c r="AD56" s="3">
+      <c r="AE56" s="3">
         <v>45173</v>
       </c>
-      <c r="AF56" s="3">
+      <c r="AG56" s="3">
         <v>45167</v>
       </c>
-      <c r="AJ56" s="3">
+      <c r="AK56" s="3">
         <v>44858</v>
       </c>
-      <c r="AK56" s="3">
+      <c r="AL56" s="3">
         <v>44888</v>
       </c>
-      <c r="BA56" s="3">
+      <c r="BG56" s="3">
         <v>44905</v>
       </c>
-      <c r="BC56" s="3">
+      <c r="BI56" s="3">
         <v>45173</v>
       </c>
     </row>
-    <row r="57" spans="1:69">
+    <row r="57" spans="1:75">
       <c r="A57" s="1">
         <v>67</v>
       </c>
@@ -9324,14 +9438,14 @@
       <c r="AA57" s="3">
         <v>45167</v>
       </c>
-      <c r="AF57" s="3">
+      <c r="AG57" s="3">
         <v>45167</v>
       </c>
-      <c r="BE57" s="3">
+      <c r="BK57" s="3">
         <v>45164</v>
       </c>
     </row>
-    <row r="58" spans="1:69">
+    <row r="58" spans="1:75">
       <c r="A58" s="1">
         <v>24</v>
       </c>
@@ -9342,7 +9456,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="59" spans="1:69">
+    <row r="59" spans="1:75">
       <c r="A59" s="1">
         <v>35</v>
       </c>
@@ -9364,20 +9478,20 @@
       <c r="AA59" s="3">
         <v>45168</v>
       </c>
-      <c r="AD59" s="3">
+      <c r="AE59" s="3">
         <v>45166</v>
       </c>
-      <c r="AF59" s="3">
+      <c r="AG59" s="3">
         <v>45168</v>
       </c>
-      <c r="BC59" s="3">
+      <c r="BI59" s="3">
         <v>45170</v>
       </c>
-      <c r="BE59" s="3">
+      <c r="BK59" s="3">
         <v>45175</v>
       </c>
     </row>
-    <row r="60" spans="1:69">
+    <row r="60" spans="1:75">
       <c r="A60" s="1">
         <v>14</v>
       </c>
@@ -9396,17 +9510,17 @@
       <c r="AA60" s="3">
         <v>45167</v>
       </c>
-      <c r="AD60" s="3">
+      <c r="AE60" s="3">
         <v>45163</v>
       </c>
-      <c r="AF60" s="3">
+      <c r="AG60" s="3">
         <v>45166</v>
       </c>
-      <c r="BC60" s="3">
+      <c r="BI60" s="3">
         <v>45171</v>
       </c>
     </row>
-    <row r="61" spans="1:69">
+    <row r="61" spans="1:75">
       <c r="A61" s="1">
         <v>25</v>
       </c>
@@ -9417,7 +9531,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:69">
+    <row r="62" spans="1:75">
       <c r="A62" s="1">
         <v>20</v>
       </c>
@@ -9436,17 +9550,17 @@
       <c r="AA62" s="3">
         <v>45160</v>
       </c>
-      <c r="AD62" s="3">
+      <c r="AE62" s="3">
         <v>45163</v>
       </c>
-      <c r="AF62" s="3">
+      <c r="AG62" s="3">
         <v>45156</v>
       </c>
-      <c r="BC62" s="3">
+      <c r="BI62" s="3">
         <v>45163</v>
       </c>
     </row>
-    <row r="63" spans="1:69">
+    <row r="63" spans="1:75">
       <c r="A63" s="1">
         <v>3</v>
       </c>
@@ -9465,20 +9579,20 @@
       <c r="AA63" s="3">
         <v>45168</v>
       </c>
-      <c r="AD63" s="3">
+      <c r="AE63" s="3">
         <v>45170</v>
       </c>
-      <c r="AF63" s="3">
+      <c r="AG63" s="3">
         <v>45168</v>
       </c>
-      <c r="BC63" s="3">
+      <c r="BI63" s="3">
         <v>45170</v>
       </c>
-      <c r="BE63" s="3">
+      <c r="BK63" s="3">
         <v>45167</v>
       </c>
     </row>
-    <row r="64" spans="1:69">
+    <row r="64" spans="1:75">
       <c r="A64" s="1">
         <v>7</v>
       </c>
@@ -9506,32 +9620,32 @@
       <c r="AA64" s="3">
         <v>45146</v>
       </c>
-      <c r="AD64" s="3">
+      <c r="AE64" s="3">
         <v>45149</v>
       </c>
-      <c r="AF64" s="3">
+      <c r="AG64" s="3">
         <v>45145</v>
       </c>
-      <c r="AX64" s="3">
+      <c r="BD64" s="3">
         <v>45195</v>
       </c>
-      <c r="BC64" s="3">
+      <c r="BI64" s="3">
         <v>45150</v>
       </c>
-      <c r="BD64" s="3">
+      <c r="BJ64" s="3">
         <v>45173</v>
       </c>
-      <c r="BE64" s="3">
+      <c r="BK64" s="3">
         <v>45187</v>
       </c>
-      <c r="BN64" s="3">
+      <c r="BT64" s="3">
         <v>45190</v>
       </c>
-      <c r="BQ64" s="3">
+      <c r="BW64" s="3">
         <v>45174</v>
       </c>
     </row>
-    <row r="65" spans="1:57">
+    <row r="65" spans="1:63">
       <c r="A65" s="1">
         <v>26</v>
       </c>
@@ -9553,20 +9667,20 @@
       <c r="AA65" s="3">
         <v>45159</v>
       </c>
-      <c r="AD65" s="3">
+      <c r="AE65" s="3">
         <v>45169</v>
       </c>
-      <c r="AF65" s="3">
+      <c r="AG65" s="3">
         <v>45157</v>
       </c>
-      <c r="BC65" s="3">
+      <c r="BI65" s="3">
         <v>45170</v>
       </c>
-      <c r="BE65" s="3">
+      <c r="BK65" s="3">
         <v>45152</v>
       </c>
     </row>
-    <row r="66" spans="1:57">
+    <row r="66" spans="1:63">
       <c r="A66" s="1">
         <v>43</v>
       </c>
@@ -9577,7 +9691,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="67" spans="1:57">
+    <row r="67" spans="1:63">
       <c r="A67" s="1">
         <v>23</v>
       </c>
@@ -9596,17 +9710,17 @@
       <c r="AA67" s="3">
         <v>45158</v>
       </c>
-      <c r="AD67" s="3">
+      <c r="AE67" s="3">
         <v>45149</v>
       </c>
-      <c r="AF67" s="3">
+      <c r="AG67" s="3">
         <v>45154</v>
       </c>
-      <c r="BC67" s="3">
+      <c r="BI67" s="3">
         <v>45159</v>
       </c>
     </row>
-    <row r="68" spans="1:57">
+    <row r="68" spans="1:63">
       <c r="A68" s="1">
         <v>50</v>
       </c>
@@ -9625,17 +9739,17 @@
       <c r="AA68" s="3">
         <v>45167</v>
       </c>
-      <c r="AD68" s="3">
+      <c r="AE68" s="3">
         <v>45168</v>
       </c>
-      <c r="AF68" s="3">
+      <c r="AG68" s="3">
         <v>45166</v>
       </c>
-      <c r="BC68" s="3">
+      <c r="BI68" s="3">
         <v>45168</v>
       </c>
     </row>
-    <row r="69" spans="1:57">
+    <row r="69" spans="1:63">
       <c r="A69" s="1">
         <v>32</v>
       </c>
@@ -9654,17 +9768,17 @@
       <c r="AA69" s="3">
         <v>45160</v>
       </c>
-      <c r="AD69" s="3">
+      <c r="AE69" s="3">
         <v>45159</v>
       </c>
-      <c r="AF69" s="3">
+      <c r="AG69" s="3">
         <v>45157</v>
       </c>
-      <c r="BC69" s="3">
+      <c r="BI69" s="3">
         <v>45168</v>
       </c>
     </row>
-    <row r="70" spans="1:57">
+    <row r="70" spans="1:63">
       <c r="A70" s="1">
         <v>71</v>
       </c>
@@ -9675,7 +9789,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="1:57">
+    <row r="71" spans="1:63">
       <c r="A71" s="1">
         <v>76</v>
       </c>
@@ -9686,7 +9800,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="72" spans="1:57">
+    <row r="72" spans="1:63">
       <c r="A72" s="1">
         <v>73</v>
       </c>
@@ -9697,7 +9811,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="73" spans="1:57">
+    <row r="73" spans="1:63">
       <c r="A73" s="1">
         <v>57</v>
       </c>
@@ -9708,7 +9822,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:57">
+    <row r="74" spans="1:63">
       <c r="A74" s="1">
         <v>74</v>
       </c>
@@ -9719,7 +9833,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="75" spans="1:57">
+    <row r="75" spans="1:63">
       <c r="A75" s="1">
         <v>53</v>
       </c>
@@ -9730,7 +9844,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:57">
+    <row r="76" spans="1:63">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -9741,7 +9855,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="1:57">
+    <row r="77" spans="1:63">
       <c r="A77" s="1">
         <v>72</v>
       </c>

</xml_diff>